<commit_message>
Added a few more genomes of IMG info
</commit_message>
<xml_diff>
--- a/Data_files/combined_genome_data.xlsx
+++ b/Data_files/combined_genome_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\MAGstravaganza\Data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amlin\Desktop\MAGstravaganza\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="545">
   <si>
     <t>ME</t>
   </si>
@@ -1608,12 +1608,63 @@
   </si>
   <si>
     <t>fructose, mannose, propanoate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carbohydrate, iron (III), multiple sugar transporter, phosphate, spermidine/putrescine, zinc, </t>
+  </si>
+  <si>
+    <t>fructose, maltose, cellubiose</t>
+  </si>
+  <si>
+    <t>No TCA cycle enzymes identified - pyruvate based metabolism?</t>
+  </si>
+  <si>
+    <t>Sulfur_oxidation(SOX)</t>
+  </si>
+  <si>
+    <t>alanine-glyoxylate, lots of amino acid transporters, glycerol-3-phosphate, carbohydrate, heme export, iron(III), molybdate, LPS export, multiple sugar transporter, phosphate, phospholipid, trehlaose/maltose, tungstate, urea</t>
+  </si>
+  <si>
+    <t>Oxidative phosphorylation, lots of acetyl-coA transferases</t>
+  </si>
+  <si>
+    <t>Motility</t>
+  </si>
+  <si>
+    <t>Flagellum (type III secretion)</t>
+  </si>
+  <si>
+    <t>lipooligosaccharide, LPS export, osmoprotectant, phosphate, phospholipid/chloresterol</t>
+  </si>
+  <si>
+    <t>Wood-Ljungdahl, polyhydroxybutryate</t>
+  </si>
+  <si>
+    <t>fructose, glycogen</t>
+  </si>
+  <si>
+    <t>Flagellum (few proteins)</t>
+  </si>
+  <si>
+    <t>Chemotaxis but no motility proteins</t>
+  </si>
+  <si>
+    <t>biotin, iron complex, iron(III), iron/zinc/copper, manganese/iron, molybdate, phsophae, spermidine/putrescine, thiamine, zinc</t>
+  </si>
+  <si>
+    <t>alkane sulfonate, taurine</t>
+  </si>
+  <si>
+    <t>Wood-Ljungdahl? (maybe just carbon monoxide + folate metabolism)</t>
+  </si>
+  <si>
+    <t>Oxidative phosphorylation, coenzyme 420 biosynthesis, lots of acetyl-CoA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2010,10 +2061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S206"/>
+  <dimension ref="A1:T206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2028,7 +2079,7 @@
     <col min="9" max="9" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
@@ -2084,10 +2135,13 @@
         <v>339</v>
       </c>
       <c r="S1" t="s">
+        <v>534</v>
+      </c>
+      <c r="T1" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2582580512</v>
       </c>
@@ -2133,8 +2187,11 @@
       <c r="Q2" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S2" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>523</v>
       </c>
@@ -2178,7 +2235,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2582580514</v>
       </c>
@@ -2207,8 +2264,20 @@
       <c r="K4" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>529</v>
+      </c>
+      <c r="N4" t="s">
+        <v>462</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>528</v>
+      </c>
+      <c r="T4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2582580515</v>
       </c>
@@ -2236,8 +2305,29 @@
       <c r="I5" s="1" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>537</v>
+      </c>
+      <c r="L5" t="s">
+        <v>368</v>
+      </c>
+      <c r="N5" t="s">
+        <v>462</v>
+      </c>
+      <c r="P5" t="s">
+        <v>531</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>532</v>
+      </c>
+      <c r="S5" t="s">
+        <v>539</v>
+      </c>
+      <c r="T5" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2582580516</v>
       </c>
@@ -2265,11 +2355,23 @@
       <c r="I6" s="1" t="s">
         <v>346</v>
       </c>
+      <c r="L6" t="s">
+        <v>538</v>
+      </c>
       <c r="M6" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>462</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>536</v>
+      </c>
+      <c r="S6" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2582580517</v>
       </c>
@@ -2297,11 +2399,26 @@
       <c r="I7" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="J7" t="s">
+        <v>543</v>
+      </c>
       <c r="M7" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N7" t="s">
+        <v>462</v>
+      </c>
+      <c r="P7" t="s">
+        <v>542</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>541</v>
+      </c>
+      <c r="T7" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2582580518</v>
       </c>
@@ -2336,7 +2453,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2582580519</v>
       </c>
@@ -2368,7 +2485,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2582580520</v>
       </c>
@@ -2397,7 +2514,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2582580521</v>
       </c>
@@ -2432,7 +2549,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2582580522</v>
       </c>
@@ -2464,7 +2581,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2582580523</v>
       </c>
@@ -2499,7 +2616,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2582580524</v>
       </c>
@@ -2534,7 +2651,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2582580525</v>
       </c>
@@ -2566,7 +2683,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2582580526</v>
       </c>

</xml_diff>

<commit_message>
Added more IMG annotations to genome table
</commit_message>
<xml_diff>
--- a/Data_files/combined_genome_data.xlsx
+++ b/Data_files/combined_genome_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amlin\Desktop\MAGstravaganza\Data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\MAGstravaganza\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="751">
   <si>
     <t>ME</t>
   </si>
@@ -1085,9 +1085,6 @@
     <t>thioadenosine</t>
   </si>
   <si>
-    <t xml:space="preserve">thioadenosine, melibiose, </t>
-  </si>
-  <si>
     <t>thioadenosine, mannose, ethanol, xylose</t>
   </si>
   <si>
@@ -1659,12 +1656,633 @@
   </si>
   <si>
     <t>Oxidative phosphorylation, coenzyme 420 biosynthesis, lots of acetyl-CoA</t>
+  </si>
+  <si>
+    <t>2582580518</t>
+  </si>
+  <si>
+    <t>glycogen, fructose</t>
+  </si>
+  <si>
+    <t>one flagellar protein, some chemotaxis</t>
+  </si>
+  <si>
+    <t>Photosynthesis, carbon fixation (RuBisCo)</t>
+  </si>
+  <si>
+    <t>nitrogen fixation, nitrite reductase</t>
+  </si>
+  <si>
+    <t>polysaccharide phosphate, methionine, arg/lys/his/glu, carbohydrate, cobalt/nickel, iron, LPS export, molybdate, neutral amino acids, phosphate, phospholipid/cholestoerol, sperimidne/putrescine, sulfate, urea</t>
+  </si>
+  <si>
+    <t>Carotenoid synthesis</t>
+  </si>
+  <si>
+    <t>branched aminos, heme export, inositol, LPS export, phosphate, phospholipid/chlosterol</t>
+  </si>
+  <si>
+    <t>ammonia_assimlation</t>
+  </si>
+  <si>
+    <t>Oxidative phosphorylation</t>
+  </si>
+  <si>
+    <t>only 1st step of sulf_red_ass</t>
+  </si>
+  <si>
+    <t>fructose, mannose, chitobiose, glucose</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, putrescine_biosynthesis</t>
+  </si>
+  <si>
+    <t>Pectin, alpha and beta glucosidases</t>
+  </si>
+  <si>
+    <t>xylose, arabinogalactan/maltooligosaccharide, branched aminos, carbohydrate, dipeptide, heme export, iron,iron (III), manganese, molybdate, multiple sugars, peptide/nickel, phosphate, spermidine/putrescine, thiamine</t>
+  </si>
+  <si>
+    <t>Oxidativephosphorylation</t>
+  </si>
+  <si>
+    <t>Two carotenoid synthesis genes, carbon monoxide dehydrogenase?, UDP-NAG, galactose</t>
+  </si>
+  <si>
+    <t>ribose/xylose/arabinose/galactoside, amino acid/amide, iron, LPS export, microcin C, monosaccarhide, oligopeptide, dipeptide, peptide/nickel, phosphate, rhamnose, spermidine/putrescine, urea, zinc/manganese</t>
+  </si>
+  <si>
+    <t>Non-melavonate terpenoid biosynthesis, oxidative phosphorylation</t>
+  </si>
+  <si>
+    <t>thioadenosine, melibiose</t>
+  </si>
+  <si>
+    <t>fructose, chitobiose, UDP-NAG, galactose, rhamnose</t>
+  </si>
+  <si>
+    <t>pectin, maltose, glycogen</t>
+  </si>
+  <si>
+    <t>dipeptide, iron, iron(III), LPS export, lipoprotein release, molybdate, monosaccharide, nitrate/nitrite, oligopeptide, peptide/nickel, phospholipid/cholesterol, phosphonate</t>
+  </si>
+  <si>
+    <t>Wood-Ljungdahl</t>
+  </si>
+  <si>
+    <t>diss_nitrate_reduction (nitrite only), ammonia_assimilation</t>
+  </si>
+  <si>
+    <t>1st half of sulf_red_ass</t>
+  </si>
+  <si>
+    <t>Flagellum and chemotaxis (ribose?)</t>
+  </si>
+  <si>
+    <t>Chitobiose, UDP-NAG, fructose, galactose, one cellulose gene, glycogen/starch</t>
+  </si>
+  <si>
+    <t>Non-melavonate terpenoid biosynthesis, oxidative phosphorylation, type II secretion</t>
+  </si>
+  <si>
+    <t>iron(III), LPS export, manganese/iron, microcin C, oligopeptide, peptide/nickel, phosphate, spermidine/putrescine</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, transport for nitrate/nitrite but no pathway</t>
+  </si>
+  <si>
+    <t>rhamnose, fructose, galactose</t>
+  </si>
+  <si>
+    <t>Lots of glucan and amylase related enzymes</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose</t>
+  </si>
+  <si>
+    <t>complete cellulose degradation!</t>
+  </si>
+  <si>
+    <t>inositol, iron, iron(III), LPS export, lipoprotein release, manganese/iron, microcin C, monosaccharide, oligopeptide, phosphate, phospolipid/cholesterol, some type II secretion genes</t>
+  </si>
+  <si>
+    <t>amino acids, biotin, carbohydrate, iron, iron(III), LPS export, manganese, nickel, nitrate, nitrate/nitrite, phosphate, phospholipid/cholesterol, phosphonate, spermidine/putrescine, urea</t>
+  </si>
+  <si>
+    <t>carbon fixation (RuBisCo)</t>
+  </si>
+  <si>
+    <t>assimilatory_nitrate_reduction, cyanate lyase</t>
+  </si>
+  <si>
+    <t>sulf_ass_red</t>
+  </si>
+  <si>
+    <t>fructose, glucose, cellulose, glycogen/starch</t>
+  </si>
+  <si>
+    <t>Oxidative phosphorylation, photosynthesis, cellulose synthase</t>
+  </si>
+  <si>
+    <t>heme, LPS export, lipoprotein release, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>glucose, mannose, cellobiose</t>
+  </si>
+  <si>
+    <t>starch/glycogen, one potential cellulose degradation gene</t>
+  </si>
+  <si>
+    <t>Phytoene synthase but no other carotenoids</t>
+  </si>
+  <si>
+    <t>xylose, amino acid/amide, biotin, branched amino, carbohydrate, glycine betaine/proline, iron, monosaccharide, phosphate, spermidine/putrescine, techoic acid</t>
+  </si>
+  <si>
+    <t>iron, LPS export, lipoprotein release, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>xylose, UDP-NAG</t>
+  </si>
+  <si>
+    <t>cobalt/nickel, iron, iron(III), LPS export, lipoprotein release, manganese/zinc/iron, molybdate, monosaccharide, phosphate, ribose, sodium, sulfate, urea, some type II secretion</t>
+  </si>
+  <si>
+    <t>flagellum, chemotaxis (ribose?)</t>
+  </si>
+  <si>
+    <t>UDP-NAG, glucose, fructose, galactose, starch/glycogen</t>
+  </si>
+  <si>
+    <t>one carotenoid gene</t>
+  </si>
+  <si>
+    <t>biotin, heme, iron, iron/zinc/copper, molybdate, nitrate/nitrite, peptide/nickel, phosphate, spermidine/putrescine, thiamine</t>
+  </si>
+  <si>
+    <t>UDP-NAG, glucose, galactose, mannose, cellobiose</t>
+  </si>
+  <si>
+    <t>amino acids, biocarbonate, biotin, branched aminos, carbohydrate, cobalt/nickel, iron (III) LPS export, molybdate, nickel, nitrate/nitrite, osmoprotectant, phsophate, phospholipid/cholesterol, chitobiose, spermidine/putrescine, sulfate, sulfonate, taurine, urea, zinc</t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, extracellular taurine, extracellular alkanesulfonate</t>
+  </si>
+  <si>
+    <t>UDP-NAG, glucose, mannose, cellobiose, starch/glycogen</t>
+  </si>
+  <si>
+    <t>heme, LPS export, lipoprotein, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>Oxidative phosphorylation, photosynthesis</t>
+  </si>
+  <si>
+    <t>one chemotaxis protein</t>
+  </si>
+  <si>
+    <t>UDP-NAG, mannose, glucose, cellobiose, sucrose</t>
+  </si>
+  <si>
+    <t>heme, LPS export, lipoprotein release, moybdae, phosphate, phospholipid/chloesterol</t>
+  </si>
+  <si>
+    <t>chitin, fructose, glucose, mannose, galactose, melibiose, pectin, starch/glycogen</t>
+  </si>
+  <si>
+    <t>carbohydrate, phosphonate, spermidine/putrescine</t>
+  </si>
+  <si>
+    <t>glucose, cellobiose</t>
+  </si>
+  <si>
+    <t>No TCA cycle, seems very streamlined w/ small genome size. Parasitic candidate phyla member? Genome completeness may be underestimated</t>
+  </si>
+  <si>
+    <t>Some carotenoid genes</t>
+  </si>
+  <si>
+    <t>branched aminos, LPS export, lipoprotein release, phospholipid/cholesterol,</t>
+  </si>
+  <si>
+    <t>chitobiose, mannose, fucose, one cellulose degradation gene</t>
+  </si>
+  <si>
+    <t>LPS export, lipoprotein release, manganese/zinc/iron, monosaccharide, osmoprotectant, phosphate, phospholipid/cholesterol, ribose, sulfate, urea</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, nitrate reductase</t>
+  </si>
+  <si>
+    <t>partial sulfate_red_ass</t>
+  </si>
+  <si>
+    <t>chemotaxis (ribose?), a flagellum specific ATPase</t>
+  </si>
+  <si>
+    <t>UDP-NAG, glucose, mannose, fructose, starch/glycogen, galacturonate</t>
+  </si>
+  <si>
+    <t>bicarbonate, biotin, branched aminos, cobalt/nickel, amino acid, iron(III), LPS export, molybdate, multiple sugar, nickel, nitrate/nitrite, oligopeptide, phosphate, phospholipid/cholesterol, chitobiose, spermidine/putrescine, sulfate, sulfonate, urea, zinc</t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, extracellular alkanesulfonate</t>
+  </si>
+  <si>
+    <t>assimilatory_nitrate_reduction, ammonia_assimilation</t>
+  </si>
+  <si>
+    <t>chemotaxis</t>
+  </si>
+  <si>
+    <t>UDP-NAG, fructose, glucose, mannose, starch/glycogen, cellobiose</t>
+  </si>
+  <si>
+    <t>Sprilloxanthin and spheroidene pathways (variants of carotenoid synthesis)</t>
+  </si>
+  <si>
+    <t>amino acid/amide, branched aminos, carbohydrate, iron (III), lipooligosaccharide, LPS export, lipoprotein release, microcin C, multiple sugars, nitrate/nitrite, oligopeptide, osmoprotectant, phosphate, phospholipid/cholesterol, g3P, tungstate, urea, type II secretion</t>
+  </si>
+  <si>
+    <t>cyanate lyase, nitroalkane, ammonia_assimilation, one nitrate reductase</t>
+  </si>
+  <si>
+    <t>sulfate oxidation, taurine, alkanesulfonate</t>
+  </si>
+  <si>
+    <t>chemotaxis (serine?), near complete flagellum with type III secretion</t>
+  </si>
+  <si>
+    <t>UDP-NAG, glycolate, starch/glycogen</t>
+  </si>
+  <si>
+    <t>amino acid/amide, biotin, branched amino, heme, iron, iron/zinc/copper, manganese, phosphate, molybdate, spermidine/putrescine, thiamine</t>
+  </si>
+  <si>
+    <t>taurine, alkanesulfonate, sulf_red_ass</t>
+  </si>
+  <si>
+    <t>Wood-Ljungdahl, acetate, galactose, UDP-NAG, cellobiose</t>
+  </si>
+  <si>
+    <t>iron (III), LPS export, lipoprotein release, manganese/zinc/iron, molybdate, monosaccharide, multiple sugar, osmoprotectant, phosphate, phospholipid/cholesterol, ribose, sodium, sulfate, type II secretion (partial)</t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, alkanesulfonate</t>
+  </si>
+  <si>
+    <t>diss_nitrate_reduction, ammonia_assimilation</t>
+  </si>
+  <si>
+    <t>flagellum with type III secretion, chemotaxis (ribose?)</t>
+  </si>
+  <si>
+    <t>chitobiose, UDP-NAG, glucose, fructose, galactose, glycolate, cellobiose, galacturonate, starch/glycogen</t>
+  </si>
+  <si>
+    <t>heme, LPS export, lipoprotein release</t>
+  </si>
+  <si>
+    <t>starch/glycogen, glucose</t>
+  </si>
+  <si>
+    <t>zinc, amino acid, LPS export, lipoprotein release, manganese/zinc/iron, monosaccharide, phosphate, phospholipid/cholesterol, sodium, urea, some type II proteins</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, one nitrate reductase</t>
+  </si>
+  <si>
+    <t>one cellulose degradation gene, starch/glycogen, glucose, chitin</t>
+  </si>
+  <si>
+    <t>iron, LPS export, lipoprotein release, phospholipid/cholesterol, phosphate</t>
+  </si>
+  <si>
+    <t>cellobiose</t>
+  </si>
+  <si>
+    <t>branched amino, amide, biotin, carbohydrate, heme, iron (III), manganese, molybdate, multiple sugar, phosphate, g3p, thiamine</t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, taurine, alkanesulfonate</t>
+  </si>
+  <si>
+    <t>UDP-NAG, glucose, mannose, lactose, galactose, glycolate, cellobiose, glycogen/starch</t>
+  </si>
+  <si>
+    <t>heme, LPS export, lipoprotein, phosphate, phospholipid/cholesterol, phosphonate</t>
+  </si>
+  <si>
+    <t>UDP-NAG, glucose, maltose</t>
+  </si>
+  <si>
+    <t>inositol, LPS export, iron, irno (III), maltose/maltodextrin, microcin C, monosaccharide, oligopeptide, phosphate, phospholipid/cholesterol, zinc/manganese, type II secretion (partial)</t>
+  </si>
+  <si>
+    <t>glycolate, UDP-NAG, glucose, fructose, cellobiose</t>
+  </si>
+  <si>
+    <t>LPS export, molybdate, lipoprotein, phosphate, ribose, sodium, type IV partial</t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, thiosulfate</t>
+  </si>
+  <si>
+    <t>Wood-Ljungdahl, acetate</t>
+  </si>
+  <si>
+    <t>chemotaxis (ribose?)</t>
+  </si>
+  <si>
+    <t>UDP-NAG, glycolate, fructose, glucose, galactose, cellulose degradation, galacturonate, maltose</t>
+  </si>
+  <si>
+    <t>heme, LPS export, lipoprotein release, phosphate, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>UDP-NAG, mannose, glycolate, cellobiose</t>
+  </si>
+  <si>
+    <t>ribose, amino acid, biotin, arabinogalactan/maltooligosaccharide, carbohydrate, branched amino, cobalamin, cobalt/nickel, fructose, iron, iron (III), LPS transport, mannose, oligopeptide, peptide/nickel, mannose, phosphate, spermidine/putrescine</t>
+  </si>
+  <si>
+    <t>maltose, glycolate, mannose, glucose</t>
+  </si>
+  <si>
+    <t>carotenoid synthesis</t>
+  </si>
+  <si>
+    <t>carotenoid synthesis, carbon fixation</t>
+  </si>
+  <si>
+    <t>nitrate_red_ass, nitrile, ammonia_assimilation</t>
+  </si>
+  <si>
+    <t>bicarbonate, biotin, carbohydrate, iron(III), LPS export, nickel, nitrate/nitrite, phsophate, phospholipid/cholesterol, phosphonate, sulfate, urea</t>
+  </si>
+  <si>
+    <t>UDP-NAG, glucose, mellobiose, glycolate, mellobiose, cellobiose, sucrose</t>
+  </si>
+  <si>
+    <t>branched amino, methionine, glutamate, histidine, amino acid, arginine/lysine/histidine/glutamine, cobatl/nickel, aspartate/glutamate, glycine betaine/choline-binding lipoprotein, iron(III), LPS export, multiple sugar, neutral amino, phosphate, phosphonate, sulfate, sulfonate, taurine, urea</t>
+  </si>
+  <si>
+    <t>one flagellar protein</t>
+  </si>
+  <si>
+    <t>starch/glycogen, cellobiose, glycolate, mannose, UDP-NAG, glucose</t>
+  </si>
+  <si>
+    <t>alpha-glucoside, arabinogalactan/maltooligosaccharide, biotin, carbohydrate, cellobiose, iron, iron(III), LPS transport, monosaccharide, phosphate, spermidine/putrescine, thiamine</t>
+  </si>
+  <si>
+    <t>maltose, cellobiose</t>
+  </si>
+  <si>
+    <t>biotin, iron, iron(III), iron/zinc/copper, manganese/zinc/iron, molybdate, phosphate, spermidine/putrescine, taurine, thiamine, zinc</t>
+  </si>
+  <si>
+    <t>alkane sulfonate, one sulfate_red_ass protein</t>
+  </si>
+  <si>
+    <t>galactose, melibiose, lactose, glucose, mannose</t>
+  </si>
+  <si>
+    <t>branched aminos, carbohydrate, cobalamin, cobalt/nickel, fructose, iron (III), mannose, phosphate, spermidine/putrescine, techoic acid</t>
+  </si>
+  <si>
+    <t>glucose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glutamate, amino acid/amide, branched aminos, carbohydrate, glutamate/aspartate, heme, phosphate, lipoprotein release, phsopholipd/cholesterol, g3p, spermidine/putrescine, tungstate, type I secretion transporter, </t>
+  </si>
+  <si>
+    <t>carbon fixation (RuBisCo), formaldehyde, acetate</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, diss_nitrate_red, some denitrification proteins</t>
+  </si>
+  <si>
+    <t>sulfate_ass_red, sulfate_diss_red, sulfate oxidation</t>
+  </si>
+  <si>
+    <t>chemotaxis (air?), flagellum, type III secretion</t>
+  </si>
+  <si>
+    <t>benzoate, fructose, glucose, glycolate, starch/glycogen</t>
+  </si>
+  <si>
+    <t>iron, iron(III), LPS export, lipoprotein release, manganese/zinc/iron, monosaccharide, osmoprotectant, phosphate, phospholipid/cholesterol, ribose, urea</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, one nitrite reductse</t>
+  </si>
+  <si>
+    <t>chemotaxis (ribose?), one flagellum protein</t>
+  </si>
+  <si>
+    <t>UDP-NAG, glucose, mannose, rhamnulose, cellulose degradation, cellobiose, starch/glycogen</t>
+  </si>
+  <si>
+    <t>nitrate/sulfonate/bicarbonate, glutamate, amino acid, amide, heme, iron (III), LPS export, lipoprotein release, microcin C, phospholipid/cholesterol, tungstate</t>
+  </si>
+  <si>
+    <t>extracellular taurine, extracellular alkanesulfonate</t>
+  </si>
+  <si>
+    <t>glycolate, chitobiose</t>
+  </si>
+  <si>
+    <t>cobalt/nickel, iron (III), LPS export, lipoprotein release, microcin C, phosphate, phospholipid/cholesterol, ribose</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, hydroxylamine reductase</t>
+  </si>
+  <si>
+    <t>sufate_red_ass</t>
+  </si>
+  <si>
+    <t>cellulose degradation, cellobiose</t>
+  </si>
+  <si>
+    <t>iron, iron(III), LPS export, lipoprotein release, manganese/zinc/iron, monosaccharide, osmoprotectant, phosphate, phospholipid/cholesterol, ribose, urea, sulfate</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, one nitrite reductase</t>
+  </si>
+  <si>
+    <t>chemotaxis (ribose?), a few flagellar proteins</t>
+  </si>
+  <si>
+    <t>UDP-NAG, glucose, mannose, fructose, rhamnulose, glycogen/starch, maltose</t>
+  </si>
+  <si>
+    <t>heme, LPS export, lipoprotein release, oligopeptide, phosphate, phospholipid/cholesterol, putrescine</t>
+  </si>
+  <si>
+    <t>methanol</t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, some sulfur oxidation</t>
+  </si>
+  <si>
+    <t>glycogen/starch, glycolate, maltose, chitobiose, glucose</t>
+  </si>
+  <si>
+    <t>two carotenoid genes</t>
+  </si>
+  <si>
+    <t>zinc</t>
+  </si>
+  <si>
+    <t>some oxidative phosphorylation</t>
+  </si>
+  <si>
+    <t>iron, heme, LPS export, lipoprotein release, phosphate, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>UDP-NAG, mannose</t>
+  </si>
+  <si>
+    <t>arabinogalactan, biotin, branched aminos, carbohydrate, cobalamin, cobalt/nickel, glucose/mannose, peptide/nickel, phosphate, spermidine/putrescine, teichoic acid</t>
+  </si>
+  <si>
+    <t>maltose, rhamulose, glucose</t>
+  </si>
+  <si>
+    <t>amino aicd/amide, biotin, branched amino, heme export, iron, iron(III), iron/zinc/copper, molybdate, monosaccharide, phosphate, peptide/nickel, spermidine/putrescine, ribose</t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, taurine</t>
+  </si>
+  <si>
+    <t>glucose, galactose, glycolate, cellobiose</t>
+  </si>
+  <si>
+    <t>branched amino, amino acid/amide, heme exort, LPS export, lipoprotein release, molybdate, phosphate, phospholipid, sulfate, urea, type II secretion</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, nitric oxide reductase</t>
+  </si>
+  <si>
+    <t>acetate, two carotenoid genes, methane, formaldehyde assimilation via serine cycle</t>
+  </si>
+  <si>
+    <t>chemotaxis (serine?), flagellum with type III secretion</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose, glycolate, cellobiose, starch/glycogen</t>
+  </si>
+  <si>
+    <t>cobalt, methionine, glutamate, amino acid/amide, bacteriocin peptidase, bicarbonate, biotin, carbohydrate, cobalamin, cobalt/nickel, LPS export, molybdate, nitrate/nitrite, osmoprotectant, phosphate, phospholipid/cholesterol, phosphonate, sulfate, urea</t>
+  </si>
+  <si>
+    <t>nitrogen fixation, nitrate_red_ass</t>
+  </si>
+  <si>
+    <t>glucose, galacturonate, maltose, starch/glycogen, glycolate, chitobiose, fructose</t>
+  </si>
+  <si>
+    <t>heme export, iron, LPS export, lipoprotein release, phosphate, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>chitin, glucose, mannose, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>amino acid, iron, iron(III), LPS export, manganese/zinc/iron, monosaccharide, phosphate, phospholipid/cholesterol, ribose, spermidine/putrescine, sodium, urea, zinc, zinc/manganese</t>
+  </si>
+  <si>
+    <t>fructose, glucose, rhamnulose, galactose, glycolate, cellulose, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>three carotenoid genes</t>
+  </si>
+  <si>
+    <t>heme export, iron, LPS export, lipoprotein release, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>squalene-hopene, oxidative phosphorylation</t>
+  </si>
+  <si>
+    <t>mannose, glycolate, cellobiose</t>
+  </si>
+  <si>
+    <t>xylose, amino acid, carbohydrate, cobalamin, cobalt/nickel, iron, iron(III), lipooligosaccharide, monosaccharide, phosphate, raffinose/stachylose/melibiose</t>
+  </si>
+  <si>
+    <t>glucose, maltose, galactose</t>
+  </si>
+  <si>
+    <t>LPS export, microcin C, peptide/nickel transport, spermidine/putrescine</t>
+  </si>
+  <si>
+    <t>UDP-NAG, galactose, glucose, fructose, rhamnulose, melibiose, stachyose, glycolate, maltose, starch/glycogen, one cellulose degradation gene</t>
+  </si>
+  <si>
+    <t>amino acid, branched amino, lipooligosaccharide, manganese/iron, oligopeptide, spermidine/putrescine</t>
+  </si>
+  <si>
+    <t>partial sulfate_red_ass, extracellular alkanesulfonate</t>
+  </si>
+  <si>
+    <t>cellobiose, UDP-NAG, glucose</t>
+  </si>
+  <si>
+    <t>ribose, biotin, branched aminos, carbohydrate, glucose/mannose, iron, iron (III), monosaccharide, neutral amino, phosphate, polar amino, rhamnose, spermidine/putrescine</t>
+  </si>
+  <si>
+    <t>glucose, rhamnose, galactose, glycolate</t>
+  </si>
+  <si>
+    <t>nitrate_red_ass, ammonia_assimilation</t>
+  </si>
+  <si>
+    <t>carbon fixation (RuBisCo), carotenoid synthesis</t>
+  </si>
+  <si>
+    <t>amino acid, bicarbonate, carbohydrate, iron, iron (III), LPS export, manganese/zinc/iron, nitrate/nitrite, osmoprotectant, phosphate, sulfate, urea</t>
+  </si>
+  <si>
+    <t>glucose, fructose, UDP-NAG, glycolate, cellulose degradation, glycogen/starch, galacturonate</t>
+  </si>
+  <si>
+    <t>amino acid, biotin, carbohydrate, capsular polysaccharide, iron (III), LPS export, manganese, nickel, phosphate, phospholipid/cholesterol, phosphonate, spermidine/putrescine, sulfate, urea</t>
+  </si>
+  <si>
+    <t>carotenoid synthesis, carbon fixation (RuBisCo)</t>
+  </si>
+  <si>
+    <t>glucose, fructose, glycolate, cellulose degradation + synthesis, galacturonate, maltose, starch/glycogen</t>
+  </si>
+  <si>
+    <t>iron, LPS export, lipoprotein, manganese/zinc/iron, monosaccharide, multiple sugar, phosphate, phospholipid/cholesterol, ribose, sodium</t>
+  </si>
+  <si>
+    <t>acetate</t>
+  </si>
+  <si>
+    <t>some chemotaxis (ribose?), some type III secretion</t>
+  </si>
+  <si>
+    <t>glucose, fructose, galactose, glycolate, glycerate, galacturonate, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>starch/glycogen, cellulose synthesis, glucose</t>
+  </si>
+  <si>
+    <t>Limited central metabolism - no TCA or nucleotide synthesis</t>
+  </si>
+  <si>
+    <t>heme, iron, lipoprotein, peptide/nickel, phosphate, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>glycolate, trehalose, maltose, cellobiose, glucose</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2063,8 +2681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T206"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="I37" workbookViewId="0">
+      <selection activeCell="L69" sqref="L69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2073,10 +2691,14 @@
     <col min="2" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="4" width="58.140625" customWidth="1"/>
     <col min="5" max="5" width="79.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" customWidth="1"/>
     <col min="9" max="9" width="20.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -2129,13 +2751,13 @@
         <v>338</v>
       </c>
       <c r="Q1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="R1" t="s">
         <v>339</v>
       </c>
       <c r="S1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="T1" t="s">
         <v>340</v>
@@ -2167,33 +2789,33 @@
         <v>342</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J2" t="s">
+        <v>519</v>
+      </c>
+      <c r="L2" t="s">
+        <v>521</v>
+      </c>
+      <c r="N2" t="s">
         <v>520</v>
       </c>
-      <c r="L2" t="s">
-        <v>522</v>
-      </c>
-      <c r="N2" t="s">
-        <v>521</v>
-      </c>
       <c r="O2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="P2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="Q2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="S2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
@@ -2219,20 +2841,23 @@
       <c r="I3" s="1" t="s">
         <v>344</v>
       </c>
+      <c r="J3" t="s">
+        <v>550</v>
+      </c>
       <c r="L3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="N3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="O3" t="s">
+        <v>502</v>
+      </c>
+      <c r="P3" t="s">
         <v>503</v>
       </c>
-      <c r="P3" t="s">
-        <v>504</v>
-      </c>
       <c r="Q3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -2265,16 +2890,16 @@
         <v>345</v>
       </c>
       <c r="L4" t="s">
+        <v>528</v>
+      </c>
+      <c r="N4" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>527</v>
+      </c>
+      <c r="T4" t="s">
         <v>529</v>
-      </c>
-      <c r="N4" t="s">
-        <v>462</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>528</v>
-      </c>
-      <c r="T4" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -2303,28 +2928,28 @@
         <v>342</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="N5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="P5" t="s">
+        <v>530</v>
+      </c>
+      <c r="Q5" t="s">
         <v>531</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="S5" t="s">
+        <v>538</v>
+      </c>
+      <c r="T5" t="s">
         <v>532</v>
-      </c>
-      <c r="S5" t="s">
-        <v>539</v>
-      </c>
-      <c r="T5" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -2356,19 +2981,19 @@
         <v>346</v>
       </c>
       <c r="L6" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="M6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="N6" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q6" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="S6" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -2397,30 +3022,30 @@
         <v>342</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J7" t="s">
+        <v>542</v>
+      </c>
+      <c r="M7" t="s">
+        <v>459</v>
+      </c>
+      <c r="N7" t="s">
+        <v>461</v>
+      </c>
+      <c r="P7" t="s">
+        <v>541</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>540</v>
+      </c>
+      <c r="T7" t="s">
         <v>543</v>
       </c>
-      <c r="M7" t="s">
-        <v>460</v>
-      </c>
-      <c r="N7" t="s">
-        <v>462</v>
-      </c>
-      <c r="P7" t="s">
-        <v>542</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>541</v>
-      </c>
-      <c r="T7" t="s">
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>544</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>2582580518</v>
       </c>
       <c r="B8" t="s">
         <v>68</v>
@@ -2446,11 +3071,29 @@
       <c r="I8" s="1" t="s">
         <v>347</v>
       </c>
+      <c r="J8" t="s">
+        <v>547</v>
+      </c>
+      <c r="L8" t="s">
+        <v>545</v>
+      </c>
       <c r="M8" t="s">
-        <v>461</v>
+        <v>460</v>
+      </c>
+      <c r="N8" t="s">
+        <v>548</v>
       </c>
       <c r="O8" t="s">
+        <v>502</v>
+      </c>
+      <c r="P8" t="s">
         <v>503</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>549</v>
+      </c>
+      <c r="S8" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -2481,8 +3124,26 @@
       <c r="I9" s="1" t="s">
         <v>349</v>
       </c>
+      <c r="J9" t="s">
+        <v>555</v>
+      </c>
+      <c r="L9" t="s">
+        <v>557</v>
+      </c>
       <c r="M9" t="s">
-        <v>462</v>
+        <v>556</v>
+      </c>
+      <c r="N9" t="s">
+        <v>552</v>
+      </c>
+      <c r="P9" t="s">
+        <v>554</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>551</v>
+      </c>
+      <c r="T9" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -2513,6 +3174,18 @@
       <c r="I10" s="1" t="s">
         <v>350</v>
       </c>
+      <c r="J10" t="s">
+        <v>560</v>
+      </c>
+      <c r="N10" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>558</v>
+      </c>
+      <c r="T10" t="s">
+        <v>559</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -2542,11 +3215,29 @@
       <c r="I11" s="1" t="s">
         <v>351</v>
       </c>
+      <c r="J11" t="s">
+        <v>564</v>
+      </c>
+      <c r="L11" t="s">
+        <v>565</v>
+      </c>
       <c r="M11" t="s">
-        <v>460</v>
+        <v>459</v>
+      </c>
+      <c r="N11" t="s">
+        <v>461</v>
       </c>
       <c r="O11" t="s">
+        <v>502</v>
+      </c>
+      <c r="P11" t="s">
         <v>503</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>561</v>
+      </c>
+      <c r="T11" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -2575,10 +3266,31 @@
         <v>342</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>353</v>
+        <v>563</v>
+      </c>
+      <c r="J12" t="s">
+        <v>567</v>
+      </c>
+      <c r="L12" t="s">
+        <v>571</v>
       </c>
       <c r="M12" t="s">
-        <v>460</v>
+        <v>459</v>
+      </c>
+      <c r="N12" t="s">
+        <v>568</v>
+      </c>
+      <c r="P12" t="s">
+        <v>569</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>566</v>
+      </c>
+      <c r="S12" t="s">
+        <v>570</v>
+      </c>
+      <c r="T12" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -2607,13 +3319,31 @@
         <v>342</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
+      </c>
+      <c r="J13" t="s">
+        <v>575</v>
+      </c>
+      <c r="L13" t="s">
+        <v>576</v>
       </c>
       <c r="M13" t="s">
-        <v>460</v>
+        <v>459</v>
+      </c>
+      <c r="N13" t="s">
+        <v>574</v>
       </c>
       <c r="O13" t="s">
-        <v>502</v>
+        <v>501</v>
+      </c>
+      <c r="P13" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>573</v>
+      </c>
+      <c r="T13" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -2642,13 +3372,31 @@
         <v>342</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
+      </c>
+      <c r="J14" t="s">
+        <v>577</v>
+      </c>
+      <c r="L14" t="s">
+        <v>578</v>
       </c>
       <c r="M14" t="s">
-        <v>463</v>
+        <v>462</v>
+      </c>
+      <c r="N14" t="s">
+        <v>461</v>
       </c>
       <c r="O14" t="s">
-        <v>504</v>
+        <v>503</v>
+      </c>
+      <c r="P14" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>579</v>
+      </c>
+      <c r="T14" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -2677,10 +3425,28 @@
         <v>342</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="J15" t="s">
+        <v>581</v>
+      </c>
+      <c r="L15" t="s">
+        <v>584</v>
       </c>
       <c r="M15" t="s">
-        <v>464</v>
+        <v>463</v>
+      </c>
+      <c r="N15" t="s">
+        <v>582</v>
+      </c>
+      <c r="P15" t="s">
+        <v>583</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>580</v>
+      </c>
+      <c r="T15" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -2709,13 +3475,25 @@
         <v>342</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
+      </c>
+      <c r="L16" t="s">
+        <v>587</v>
+      </c>
+      <c r="N16" t="s">
+        <v>461</v>
       </c>
       <c r="O16" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>586</v>
+      </c>
+      <c r="T16" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2582580527</v>
       </c>
@@ -2741,13 +3519,28 @@
         <v>342</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
+      </c>
+      <c r="J17" t="s">
+        <v>550</v>
+      </c>
+      <c r="L17" t="s">
+        <v>588</v>
+      </c>
+      <c r="N17" t="s">
+        <v>461</v>
       </c>
       <c r="O17" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>591</v>
+      </c>
+      <c r="T17" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2582580528</v>
       </c>
@@ -2773,10 +3566,25 @@
         <v>342</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+      <c r="J18" t="s">
+        <v>589</v>
+      </c>
+      <c r="L18" t="s">
+        <v>592</v>
+      </c>
+      <c r="N18" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>590</v>
+      </c>
+      <c r="T18" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2582580529</v>
       </c>
@@ -2802,13 +3610,28 @@
         <v>342</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
+      </c>
+      <c r="L19" t="s">
+        <v>595</v>
+      </c>
+      <c r="N19" t="s">
+        <v>461</v>
       </c>
       <c r="O19" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+        <v>504</v>
+      </c>
+      <c r="P19" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>593</v>
+      </c>
+      <c r="S19" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2582580530</v>
       </c>
@@ -2834,10 +3657,25 @@
         <v>342</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+      <c r="J20" t="s">
+        <v>596</v>
+      </c>
+      <c r="L20" t="s">
+        <v>598</v>
+      </c>
+      <c r="N20" t="s">
+        <v>574</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>597</v>
+      </c>
+      <c r="T20" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2582580531</v>
       </c>
@@ -2863,16 +3701,34 @@
         <v>342</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
+      </c>
+      <c r="J21" t="s">
+        <v>581</v>
+      </c>
+      <c r="L21" t="s">
+        <v>601</v>
       </c>
       <c r="M21" t="s">
-        <v>465</v>
+        <v>464</v>
+      </c>
+      <c r="N21" t="s">
+        <v>461</v>
       </c>
       <c r="O21" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+        <v>505</v>
+      </c>
+      <c r="P21" t="s">
+        <v>600</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>599</v>
+      </c>
+      <c r="T21" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2582580532</v>
       </c>
@@ -2898,16 +3754,34 @@
         <v>342</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
+      </c>
+      <c r="J22" t="s">
+        <v>550</v>
+      </c>
+      <c r="L22" t="s">
+        <v>607</v>
       </c>
       <c r="M22" t="s">
-        <v>460</v>
+        <v>459</v>
+      </c>
+      <c r="N22" t="s">
+        <v>461</v>
       </c>
       <c r="O22" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>606</v>
+      </c>
+      <c r="S22" t="s">
+        <v>604</v>
+      </c>
+      <c r="T22" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2582580533</v>
       </c>
@@ -2933,10 +3807,25 @@
         <v>342</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+      <c r="L23" t="s">
+        <v>605</v>
+      </c>
+      <c r="N23" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>602</v>
+      </c>
+      <c r="S23" t="s">
+        <v>604</v>
+      </c>
+      <c r="T23" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2582580534</v>
       </c>
@@ -2962,10 +3851,22 @@
         <v>342</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+      <c r="L24" t="s">
+        <v>609</v>
+      </c>
+      <c r="N24" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>608</v>
+      </c>
+      <c r="T24" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2582580535</v>
       </c>
@@ -2991,13 +3892,34 @@
         <v>342</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
+      </c>
+      <c r="J25" t="s">
+        <v>611</v>
+      </c>
+      <c r="L25" t="s">
+        <v>613</v>
       </c>
       <c r="M25" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+      <c r="N25" t="s">
+        <v>461</v>
+      </c>
+      <c r="P25" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>612</v>
+      </c>
+      <c r="S25" t="s">
+        <v>604</v>
+      </c>
+      <c r="T25" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2582580536</v>
       </c>
@@ -3023,13 +3945,31 @@
         <v>342</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
+      </c>
+      <c r="L26" t="s">
+        <v>618</v>
       </c>
       <c r="M26" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+        <v>458</v>
+      </c>
+      <c r="N26" t="s">
+        <v>615</v>
+      </c>
+      <c r="P26" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>614</v>
+      </c>
+      <c r="S26" t="s">
+        <v>617</v>
+      </c>
+      <c r="T26" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2582580537</v>
       </c>
@@ -3057,11 +3997,32 @@
       <c r="I27" s="1" t="s">
         <v>352</v>
       </c>
+      <c r="J27" t="s">
+        <v>550</v>
+      </c>
+      <c r="L27" t="s">
+        <v>623</v>
+      </c>
       <c r="M27" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+        <v>466</v>
+      </c>
+      <c r="N27" t="s">
+        <v>621</v>
+      </c>
+      <c r="P27" t="s">
+        <v>620</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>619</v>
+      </c>
+      <c r="S27" t="s">
+        <v>622</v>
+      </c>
+      <c r="T27" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2582580538</v>
       </c>
@@ -3087,16 +4048,37 @@
         <v>342</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
+      </c>
+      <c r="J28" t="s">
+        <v>567</v>
       </c>
       <c r="K28" t="s">
         <v>345</v>
       </c>
+      <c r="L28" t="s">
+        <v>629</v>
+      </c>
+      <c r="N28" t="s">
+        <v>626</v>
+      </c>
       <c r="O28" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+      <c r="P28" t="s">
+        <v>627</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>625</v>
+      </c>
+      <c r="S28" t="s">
+        <v>628</v>
+      </c>
+      <c r="T28" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2582580539</v>
       </c>
@@ -3122,10 +4104,19 @@
         <v>342</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+      <c r="J29" t="s">
+        <v>632</v>
+      </c>
+      <c r="P29" t="s">
+        <v>631</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2582580540</v>
       </c>
@@ -3151,16 +4142,34 @@
         <v>342</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
+      </c>
+      <c r="J30" t="s">
+        <v>637</v>
       </c>
       <c r="M30" t="s">
-        <v>468</v>
+        <v>467</v>
+      </c>
+      <c r="N30" t="s">
+        <v>635</v>
       </c>
       <c r="O30" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+        <v>503</v>
+      </c>
+      <c r="P30" t="s">
+        <v>634</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>633</v>
+      </c>
+      <c r="S30" t="s">
+        <v>636</v>
+      </c>
+      <c r="T30" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2582580541</v>
       </c>
@@ -3186,13 +4195,31 @@
         <v>342</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
+      </c>
+      <c r="J31" t="s">
+        <v>550</v>
+      </c>
+      <c r="L31" t="s">
+        <v>639</v>
       </c>
       <c r="M31" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+        <v>468</v>
+      </c>
+      <c r="N31" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>638</v>
+      </c>
+      <c r="S31" t="s">
+        <v>604</v>
+      </c>
+      <c r="T31" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2582580542</v>
       </c>
@@ -3218,13 +4245,28 @@
         <v>342</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
+      </c>
+      <c r="L32" t="s">
+        <v>642</v>
       </c>
       <c r="M32" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+      <c r="N32" t="s">
+        <v>641</v>
+      </c>
+      <c r="P32" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>640</v>
+      </c>
+      <c r="T32" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2582580543</v>
       </c>
@@ -3250,8 +4292,20 @@
         <v>342</v>
       </c>
       <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L33" t="s">
+        <v>644</v>
+      </c>
+      <c r="N33" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>643</v>
+      </c>
+      <c r="T33" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2582580544</v>
       </c>
@@ -3277,10 +4331,25 @@
         <v>342</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+      <c r="L34" t="s">
+        <v>647</v>
+      </c>
+      <c r="N34" t="s">
+        <v>641</v>
+      </c>
+      <c r="P34" t="s">
+        <v>646</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>645</v>
+      </c>
+      <c r="T34" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2582580545</v>
       </c>
@@ -3306,13 +4375,22 @@
         <v>342</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
+      </c>
+      <c r="L35" t="s">
+        <v>649</v>
       </c>
       <c r="M35" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>648</v>
+      </c>
+      <c r="T35" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2582580546</v>
       </c>
@@ -3338,13 +4416,25 @@
         <v>342</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
+      </c>
+      <c r="L36" t="s">
+        <v>651</v>
       </c>
       <c r="M36" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+        <v>470</v>
+      </c>
+      <c r="N36" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>650</v>
+      </c>
+      <c r="T36" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2582580547</v>
       </c>
@@ -3372,11 +4462,32 @@
       <c r="I37" s="1" t="s">
         <v>343</v>
       </c>
+      <c r="J37" t="s">
+        <v>654</v>
+      </c>
+      <c r="L37" t="s">
+        <v>656</v>
+      </c>
+      <c r="N37" t="s">
+        <v>641</v>
+      </c>
       <c r="O37" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+      <c r="P37" t="s">
+        <v>653</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>652</v>
+      </c>
+      <c r="S37" t="s">
+        <v>655</v>
+      </c>
+      <c r="T37" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2582580548</v>
       </c>
@@ -3402,13 +4513,31 @@
         <v>342</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
+      </c>
+      <c r="L38" t="s">
+        <v>629</v>
       </c>
       <c r="M38" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+      <c r="N38" t="s">
+        <v>461</v>
+      </c>
+      <c r="O38" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>657</v>
+      </c>
+      <c r="S38" t="s">
+        <v>604</v>
+      </c>
+      <c r="T38" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2582580549</v>
       </c>
@@ -3434,10 +4563,25 @@
         <v>342</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+      <c r="L39" t="s">
+        <v>658</v>
+      </c>
+      <c r="N39" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>643</v>
+      </c>
+      <c r="S39" t="s">
+        <v>604</v>
+      </c>
+      <c r="T39" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2582580550</v>
       </c>
@@ -3463,16 +4607,31 @@
         <v>342</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
+      </c>
+      <c r="J40" t="s">
+        <v>596</v>
+      </c>
+      <c r="K40" t="s">
+        <v>660</v>
       </c>
       <c r="M40" t="s">
-        <v>472</v>
+        <v>471</v>
+      </c>
+      <c r="N40" t="s">
+        <v>461</v>
       </c>
       <c r="O40" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>659</v>
+      </c>
+      <c r="T40" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2582580551</v>
       </c>
@@ -3498,13 +4657,34 @@
         <v>342</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
+      </c>
+      <c r="J41" t="s">
+        <v>662</v>
+      </c>
+      <c r="L41" t="s">
+        <v>665</v>
       </c>
       <c r="M41" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+        <v>463</v>
+      </c>
+      <c r="O41" t="s">
+        <v>663</v>
+      </c>
+      <c r="P41" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>664</v>
+      </c>
+      <c r="S41" t="s">
+        <v>604</v>
+      </c>
+      <c r="T41" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2582580552</v>
       </c>
@@ -3532,11 +4712,32 @@
       <c r="I42" s="1" t="s">
         <v>346</v>
       </c>
+      <c r="J42" t="s">
+        <v>662</v>
+      </c>
+      <c r="L42" t="s">
+        <v>668</v>
+      </c>
       <c r="M42" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+        <v>472</v>
+      </c>
+      <c r="N42" t="s">
+        <v>461</v>
+      </c>
+      <c r="P42" t="s">
+        <v>600</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>666</v>
+      </c>
+      <c r="S42" t="s">
+        <v>667</v>
+      </c>
+      <c r="T42" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2582580553</v>
       </c>
@@ -3562,8 +4763,20 @@
         <v>342</v>
       </c>
       <c r="I43" s="1"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L43" t="s">
+        <v>670</v>
+      </c>
+      <c r="N43" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>669</v>
+      </c>
+      <c r="T43" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>2582580554</v>
       </c>
@@ -3589,11 +4802,26 @@
         <v>342</v>
       </c>
       <c r="I44" s="1"/>
+      <c r="L44" t="s">
+        <v>673</v>
+      </c>
+      <c r="N44" t="s">
+        <v>461</v>
+      </c>
       <c r="O44" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+      <c r="P44" t="s">
+        <v>672</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>671</v>
+      </c>
+      <c r="T44" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2582580555</v>
       </c>
@@ -3619,10 +4847,19 @@
         <v>342</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+      <c r="K45" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>674</v>
+      </c>
+      <c r="T45" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>2582580556</v>
       </c>
@@ -3648,16 +4885,37 @@
         <v>342</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
+      </c>
+      <c r="J46" t="s">
+        <v>677</v>
+      </c>
+      <c r="L46" t="s">
+        <v>681</v>
       </c>
       <c r="M46" t="s">
-        <v>474</v>
+        <v>473</v>
+      </c>
+      <c r="N46" t="s">
+        <v>678</v>
       </c>
       <c r="O46" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+        <v>506</v>
+      </c>
+      <c r="P46" t="s">
+        <v>679</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>676</v>
+      </c>
+      <c r="S46" t="s">
+        <v>680</v>
+      </c>
+      <c r="T46" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>2582580557</v>
       </c>
@@ -3683,8 +4941,29 @@
         <v>342</v>
       </c>
       <c r="I47" s="1"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J47" t="s">
+        <v>661</v>
+      </c>
+      <c r="L47" t="s">
+        <v>688</v>
+      </c>
+      <c r="N47" t="s">
+        <v>461</v>
+      </c>
+      <c r="P47" t="s">
+        <v>687</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>686</v>
+      </c>
+      <c r="S47" t="s">
+        <v>667</v>
+      </c>
+      <c r="T47" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>2582580558</v>
       </c>
@@ -3710,13 +4989,31 @@
         <v>342</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
+      </c>
+      <c r="J48" t="s">
+        <v>661</v>
+      </c>
+      <c r="L48" t="s">
+        <v>685</v>
       </c>
       <c r="M48" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+        <v>471</v>
+      </c>
+      <c r="N48" t="s">
+        <v>683</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>682</v>
+      </c>
+      <c r="S48" t="s">
+        <v>684</v>
+      </c>
+      <c r="T48" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>2582580559</v>
       </c>
@@ -3742,10 +5039,22 @@
         <v>342</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+      <c r="M49" t="s">
+        <v>692</v>
+      </c>
+      <c r="N49" t="s">
+        <v>690</v>
+      </c>
+      <c r="P49" t="s">
+        <v>691</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>2582580560</v>
       </c>
@@ -3771,16 +5080,34 @@
         <v>342</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
+      </c>
+      <c r="K50" t="s">
+        <v>696</v>
       </c>
       <c r="M50" t="s">
-        <v>475</v>
+        <v>474</v>
+      </c>
+      <c r="N50" t="s">
+        <v>694</v>
       </c>
       <c r="O50" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+        <v>501</v>
+      </c>
+      <c r="P50" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>693</v>
+      </c>
+      <c r="S50" t="s">
+        <v>695</v>
+      </c>
+      <c r="T50" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>2582580561</v>
       </c>
@@ -3806,16 +5133,34 @@
         <v>342</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
+      </c>
+      <c r="J51" t="s">
+        <v>698</v>
+      </c>
+      <c r="K51" t="s">
+        <v>700</v>
       </c>
       <c r="M51" t="s">
-        <v>460</v>
+        <v>459</v>
+      </c>
+      <c r="N51" t="s">
+        <v>461</v>
       </c>
       <c r="O51" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+        <v>501</v>
+      </c>
+      <c r="P51" t="s">
+        <v>699</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>697</v>
+      </c>
+      <c r="T51" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>2582580562</v>
       </c>
@@ -3841,8 +5186,17 @@
         <v>342</v>
       </c>
       <c r="I52" s="1"/>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J52" t="s">
+        <v>701</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>702</v>
+      </c>
+      <c r="T52" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>2582580563</v>
       </c>
@@ -3868,11 +5222,29 @@
         <v>342</v>
       </c>
       <c r="I53" s="1"/>
+      <c r="J53" t="s">
+        <v>701</v>
+      </c>
+      <c r="L53" t="s">
+        <v>705</v>
+      </c>
+      <c r="N53" t="s">
+        <v>461</v>
+      </c>
       <c r="O53" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+      <c r="P53" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>704</v>
+      </c>
+      <c r="T53" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>2582580564</v>
       </c>
@@ -3898,10 +5270,28 @@
         <v>342</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+      <c r="J54" t="s">
+        <v>701</v>
+      </c>
+      <c r="L54" t="s">
+        <v>707</v>
+      </c>
+      <c r="N54" t="s">
+        <v>461</v>
+      </c>
+      <c r="P54" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>706</v>
+      </c>
+      <c r="T54" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>2582580565</v>
       </c>
@@ -3927,16 +5317,34 @@
         <v>342</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
+      </c>
+      <c r="J55" t="s">
+        <v>567</v>
+      </c>
+      <c r="L55" t="s">
+        <v>710</v>
       </c>
       <c r="M55" t="s">
-        <v>476</v>
+        <v>475</v>
+      </c>
+      <c r="N55" t="s">
+        <v>461</v>
       </c>
       <c r="O55" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+        <v>507</v>
+      </c>
+      <c r="P55" t="s">
+        <v>709</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>708</v>
+      </c>
+      <c r="T55" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>2582580566</v>
       </c>
@@ -3962,16 +5370,37 @@
         <v>342</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
+      </c>
+      <c r="J56" t="s">
+        <v>713</v>
+      </c>
+      <c r="L56" t="s">
+        <v>715</v>
       </c>
       <c r="M56" t="s">
-        <v>477</v>
+        <v>476</v>
+      </c>
+      <c r="N56" t="s">
+        <v>712</v>
       </c>
       <c r="O56" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+        <v>501</v>
+      </c>
+      <c r="P56" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>711</v>
+      </c>
+      <c r="S56" t="s">
+        <v>714</v>
+      </c>
+      <c r="T56" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>2582580567</v>
       </c>
@@ -3997,13 +5426,28 @@
         <v>342</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
+      </c>
+      <c r="J57" t="s">
+        <v>662</v>
+      </c>
+      <c r="L57" t="s">
+        <v>718</v>
       </c>
       <c r="M57" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>477</v>
+      </c>
+      <c r="N57" t="s">
+        <v>717</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>716</v>
+      </c>
+      <c r="T57" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>2582580568</v>
       </c>
@@ -4029,13 +5473,31 @@
         <v>342</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
+      </c>
+      <c r="J58" t="s">
+        <v>661</v>
+      </c>
+      <c r="L58" t="s">
+        <v>720</v>
       </c>
       <c r="M58" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>469</v>
+      </c>
+      <c r="N58" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>719</v>
+      </c>
+      <c r="S58" t="s">
+        <v>604</v>
+      </c>
+      <c r="T58" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>2582580569</v>
       </c>
@@ -4061,19 +5523,38 @@
         <v>342</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
+        <v>428</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="K59" t="s">
+        <v>722</v>
+      </c>
       <c r="L59" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="M59" s="4"/>
+      <c r="N59" t="s">
+        <v>461</v>
+      </c>
       <c r="O59" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+        <v>501</v>
+      </c>
+      <c r="P59" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>721</v>
+      </c>
+      <c r="S59" t="s">
+        <v>655</v>
+      </c>
+      <c r="T59" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>2582580571</v>
       </c>
@@ -4099,13 +5580,28 @@
         <v>342</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
+      </c>
+      <c r="J60" t="s">
+        <v>723</v>
+      </c>
+      <c r="L60" t="s">
+        <v>726</v>
       </c>
       <c r="M60" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+      <c r="N60" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>724</v>
+      </c>
+      <c r="T60" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>2582580572</v>
       </c>
@@ -4133,8 +5629,20 @@
       <c r="I61" s="1" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L61" t="s">
+        <v>728</v>
+      </c>
+      <c r="N61" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>727</v>
+      </c>
+      <c r="T61" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>2582580573</v>
       </c>
@@ -4160,10 +5668,25 @@
         <v>342</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+      <c r="K62" t="s">
+        <v>730</v>
+      </c>
+      <c r="N62" t="s">
+        <v>461</v>
+      </c>
+      <c r="P62" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>729</v>
+      </c>
+      <c r="T62" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>2582580574</v>
       </c>
@@ -4189,10 +5712,28 @@
         <v>342</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+      <c r="J63" t="s">
+        <v>701</v>
+      </c>
+      <c r="L63" t="s">
+        <v>733</v>
+      </c>
+      <c r="N63" t="s">
+        <v>461</v>
+      </c>
+      <c r="P63" t="s">
+        <v>732</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>731</v>
+      </c>
+      <c r="T63" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>2582580575</v>
       </c>
@@ -4218,10 +5759,28 @@
         <v>342</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+      <c r="J64" t="s">
+        <v>701</v>
+      </c>
+      <c r="L64" t="s">
+        <v>735</v>
+      </c>
+      <c r="N64" t="s">
+        <v>461</v>
+      </c>
+      <c r="P64" t="s">
+        <v>732</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>734</v>
+      </c>
+      <c r="T64" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>2582580576</v>
       </c>
@@ -4247,13 +5806,34 @@
         <v>342</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="J65" t="s">
+        <v>737</v>
+      </c>
+      <c r="L65" t="s">
+        <v>739</v>
       </c>
       <c r="M65" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+        <v>463</v>
+      </c>
+      <c r="N65" t="s">
+        <v>736</v>
+      </c>
+      <c r="P65" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>738</v>
+      </c>
+      <c r="S65" t="s">
+        <v>604</v>
+      </c>
+      <c r="T65" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>2582580577</v>
       </c>
@@ -4281,11 +5861,29 @@
       <c r="I66" s="1" t="s">
         <v>346</v>
       </c>
+      <c r="J66" t="s">
+        <v>741</v>
+      </c>
+      <c r="L66" t="s">
+        <v>742</v>
+      </c>
       <c r="M66" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+        <v>471</v>
+      </c>
+      <c r="N66" t="s">
+        <v>461</v>
+      </c>
+      <c r="P66" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>740</v>
+      </c>
+      <c r="T66" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>2582580578</v>
       </c>
@@ -4311,16 +5909,37 @@
         <v>342</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
+      </c>
+      <c r="J67" t="s">
+        <v>744</v>
+      </c>
+      <c r="L67" t="s">
+        <v>746</v>
       </c>
       <c r="M67" t="s">
-        <v>479</v>
+        <v>478</v>
+      </c>
+      <c r="N67" t="s">
+        <v>641</v>
       </c>
       <c r="O67" t="s">
+        <v>502</v>
+      </c>
+      <c r="P67" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q67" t="s">
+        <v>743</v>
+      </c>
+      <c r="S67" t="s">
+        <v>745</v>
+      </c>
+      <c r="T67" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>2582580579</v>
       </c>
@@ -4346,10 +5965,19 @@
         <v>342</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+      <c r="L68" t="s">
+        <v>747</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>702</v>
+      </c>
+      <c r="T68" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>2582580580</v>
       </c>
@@ -4375,10 +6003,25 @@
         <v>342</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+      <c r="J69" t="s">
+        <v>611</v>
+      </c>
+      <c r="L69" t="s">
+        <v>750</v>
+      </c>
+      <c r="N69" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>749</v>
+      </c>
+      <c r="T69" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>2582580581</v>
       </c>
@@ -4404,13 +6047,13 @@
         <v>342</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="K70" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>2582580582</v>
       </c>
@@ -4436,10 +6079,10 @@
         <v>342</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>2582580583</v>
       </c>
@@ -4465,10 +6108,10 @@
         <v>342</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>2582580584</v>
       </c>
@@ -4494,13 +6137,13 @@
         <v>342</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="M73" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>2582580585</v>
       </c>
@@ -4526,13 +6169,13 @@
         <v>342</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="M74" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>2582580586</v>
       </c>
@@ -4558,13 +6201,13 @@
         <v>342</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="M75" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>2582580587</v>
       </c>
@@ -4591,7 +6234,7 @@
       </c>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>2582580588</v>
       </c>
@@ -4617,10 +6260,10 @@
         <v>342</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>2582580589</v>
       </c>
@@ -4646,13 +6289,13 @@
         <v>342</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="M78" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>2582580590</v>
       </c>
@@ -4678,10 +6321,10 @@
         <v>342</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>2582580591</v>
       </c>
@@ -4736,7 +6379,7 @@
         <v>342</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
@@ -4765,10 +6408,10 @@
         <v>342</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="O82" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
@@ -4824,10 +6467,10 @@
         <v>342</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="O84" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
@@ -4856,10 +6499,10 @@
         <v>342</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="M85" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
@@ -4888,7 +6531,7 @@
         <v>342</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
@@ -4946,10 +6589,10 @@
         <v>342</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="M88" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
@@ -4978,16 +6621,16 @@
         <v>342</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="K89" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="M89" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="O89" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
@@ -5016,13 +6659,13 @@
         <v>342</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M90" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="O90" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
@@ -5051,7 +6694,7 @@
         <v>342</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
@@ -5080,13 +6723,13 @@
         <v>342</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="M92" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="O92" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
@@ -5142,10 +6785,10 @@
         <v>342</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="M94" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
@@ -5174,13 +6817,13 @@
         <v>342</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="M95" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="O95" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
@@ -5209,13 +6852,13 @@
         <v>342</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="M96" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="O96" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
@@ -5273,7 +6916,7 @@
         <v>342</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
@@ -5329,13 +6972,13 @@
         <v>342</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="M100" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O100" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
@@ -5365,10 +7008,10 @@
       </c>
       <c r="I101" s="1"/>
       <c r="M101" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="O101" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
@@ -5397,13 +7040,13 @@
         <v>342</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="M102" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="O102" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
@@ -5432,10 +7075,10 @@
         <v>342</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="O103" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
@@ -5464,13 +7107,13 @@
         <v>2593339178</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="M104" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="O104" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
@@ -5500,7 +7143,7 @@
       </c>
       <c r="I105" s="1"/>
       <c r="M105" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
@@ -5556,13 +7199,13 @@
         <v>2593339177</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="M107" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="O107" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
@@ -5591,13 +7234,13 @@
         <v>342</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K108" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="O108" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
@@ -5626,13 +7269,13 @@
         <v>2582580651</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="M109" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="O109" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
@@ -5661,10 +7304,10 @@
         <v>2593339176</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="M110" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
@@ -5694,7 +7337,7 @@
       </c>
       <c r="I111" s="1"/>
       <c r="M111" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
@@ -5724,10 +7367,10 @@
       </c>
       <c r="I112" s="1"/>
       <c r="M112" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O112" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
@@ -5756,13 +7399,13 @@
         <v>2582580705</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="M113" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O113" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
@@ -5791,7 +7434,7 @@
         <v>2582580670</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.25">
@@ -5821,7 +7464,7 @@
       </c>
       <c r="I115" s="1"/>
       <c r="M115" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.25">
@@ -5850,10 +7493,10 @@
         <v>2582580675</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M116" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
@@ -5882,7 +7525,7 @@
         <v>342</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
@@ -5911,7 +7554,7 @@
         <v>342</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.25">
@@ -6028,10 +7671,10 @@
         <v>2582580653</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="O122" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.25">
@@ -6060,13 +7703,13 @@
         <v>342</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="M123" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="O123" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.25">
@@ -6095,10 +7738,10 @@
         <v>2593339191</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="O124" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.25">
@@ -6127,13 +7770,13 @@
         <v>342</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M125" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="O125" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.25">
@@ -6162,10 +7805,10 @@
         <v>342</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="O126" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.25">
@@ -6198,7 +7841,7 @@
         <v>345</v>
       </c>
       <c r="O127" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.25">
@@ -6281,13 +7924,13 @@
         <v>342</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="M130" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="O130" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.25">
@@ -6316,7 +7959,7 @@
         <v>342</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.25">
@@ -6345,13 +7988,13 @@
         <v>2582580662</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="M132" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="O132" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.25">
@@ -6380,10 +8023,10 @@
         <v>2593339182</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="M133" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.25">
@@ -6412,13 +8055,13 @@
         <v>342</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="M134" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="O134" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.25">
@@ -6447,13 +8090,13 @@
         <v>2582580622</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="M135" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="O135" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.25">
@@ -6482,7 +8125,7 @@
         <v>342</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.25">
@@ -6511,10 +8154,10 @@
         <v>2582580637</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="O137" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="138" spans="1:15" x14ac:dyDescent="0.25">
@@ -6543,13 +8186,13 @@
         <v>342</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="M138" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="O138" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.25">
@@ -6578,10 +8221,10 @@
         <v>342</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="M139" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="140" spans="1:15" x14ac:dyDescent="0.25">
@@ -6610,13 +8253,13 @@
         <v>342</v>
       </c>
       <c r="I140" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="K140" t="s">
         <v>399</v>
       </c>
-      <c r="K140" t="s">
-        <v>400</v>
-      </c>
       <c r="O140" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="141" spans="1:15" x14ac:dyDescent="0.25">
@@ -6645,16 +8288,16 @@
         <v>342</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="K141" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="M141" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O141" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="142" spans="1:15" x14ac:dyDescent="0.25">
@@ -6683,10 +8326,10 @@
         <v>2582580648</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="O142" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="143" spans="1:15" x14ac:dyDescent="0.25">
@@ -6742,10 +8385,10 @@
         <v>342</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="M144" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="145" spans="1:15" x14ac:dyDescent="0.25">
@@ -6774,13 +8417,13 @@
         <v>342</v>
       </c>
       <c r="I145" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="M145" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="O145" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="146" spans="1:15" x14ac:dyDescent="0.25">
@@ -6809,13 +8452,13 @@
         <v>342</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="M146" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="O146" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="147" spans="1:15" x14ac:dyDescent="0.25">
@@ -6844,13 +8487,13 @@
         <v>342</v>
       </c>
       <c r="I147" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="M147" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="O147" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="148" spans="1:15" x14ac:dyDescent="0.25">
@@ -6908,7 +8551,7 @@
         <v>2582580617</v>
       </c>
       <c r="I149" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="150" spans="1:15" x14ac:dyDescent="0.25">
@@ -6937,13 +8580,13 @@
         <v>342</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="M150" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="O150" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="151" spans="1:15" x14ac:dyDescent="0.25">
@@ -6972,10 +8615,10 @@
         <v>342</v>
       </c>
       <c r="I151" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="O151" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="152" spans="1:15" x14ac:dyDescent="0.25">
@@ -7004,10 +8647,10 @@
         <v>342</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="O152" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="153" spans="1:15" x14ac:dyDescent="0.25">
@@ -7036,10 +8679,10 @@
         <v>2582580630</v>
       </c>
       <c r="I153" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="O153" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="154" spans="1:15" x14ac:dyDescent="0.25">
@@ -7068,13 +8711,13 @@
         <v>342</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M154" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O154" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="155" spans="1:15" x14ac:dyDescent="0.25">
@@ -7130,13 +8773,13 @@
         <v>342</v>
       </c>
       <c r="I156" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="M156" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O156" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="157" spans="1:15" x14ac:dyDescent="0.25">
@@ -7165,10 +8808,10 @@
         <v>342</v>
       </c>
       <c r="I157" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M157" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.25">
@@ -7198,7 +8841,7 @@
       </c>
       <c r="I158" s="1"/>
       <c r="M158" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="159" spans="1:15" x14ac:dyDescent="0.25">
@@ -7228,7 +8871,7 @@
       </c>
       <c r="I159" s="1"/>
       <c r="O159" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="160" spans="1:15" x14ac:dyDescent="0.25">
@@ -7257,7 +8900,7 @@
         <v>342</v>
       </c>
       <c r="I160" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="161" spans="1:15" x14ac:dyDescent="0.25">
@@ -7286,7 +8929,7 @@
         <v>342</v>
       </c>
       <c r="I161" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="162" spans="1:15" x14ac:dyDescent="0.25">
@@ -7315,13 +8958,13 @@
         <v>342</v>
       </c>
       <c r="I162" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="M162" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="O162" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="163" spans="1:15" x14ac:dyDescent="0.25">
@@ -7350,10 +8993,10 @@
         <v>342</v>
       </c>
       <c r="I163" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="O163" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="164" spans="1:15" x14ac:dyDescent="0.25">
@@ -7385,10 +9028,10 @@
         <v>346</v>
       </c>
       <c r="M164" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="O164" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="165" spans="1:15" x14ac:dyDescent="0.25">
@@ -7417,7 +9060,7 @@
         <v>342</v>
       </c>
       <c r="I165" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="166" spans="1:15" x14ac:dyDescent="0.25">
@@ -7446,13 +9089,13 @@
         <v>342</v>
       </c>
       <c r="I166" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M166" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="O166" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="167" spans="1:15" x14ac:dyDescent="0.25">
@@ -7481,10 +9124,10 @@
         <v>342</v>
       </c>
       <c r="I167" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="M167" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="168" spans="1:15" x14ac:dyDescent="0.25">
@@ -7567,13 +9210,13 @@
         <v>342</v>
       </c>
       <c r="I170" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="M170" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="O170" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="171" spans="1:15" x14ac:dyDescent="0.25">
@@ -7602,13 +9245,13 @@
         <v>342</v>
       </c>
       <c r="I171" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="M171" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="O171" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="172" spans="1:15" x14ac:dyDescent="0.25">
@@ -7665,7 +9308,7 @@
       </c>
       <c r="I173" s="1"/>
       <c r="M173" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="174" spans="1:15" x14ac:dyDescent="0.25">
@@ -7695,10 +9338,10 @@
       </c>
       <c r="I174" s="1"/>
       <c r="K174" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="O174" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="175" spans="1:15" x14ac:dyDescent="0.25">
@@ -7754,13 +9397,13 @@
         <v>342</v>
       </c>
       <c r="I176" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="M176" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="O176" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="177" spans="1:15" x14ac:dyDescent="0.25">
@@ -7789,10 +9432,10 @@
         <v>342</v>
       </c>
       <c r="I177" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="M177" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="178" spans="1:15" x14ac:dyDescent="0.25">
@@ -7848,10 +9491,10 @@
         <v>2582580627</v>
       </c>
       <c r="I179" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="O179" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.25">
@@ -7907,13 +9550,13 @@
         <v>342</v>
       </c>
       <c r="I181" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="M181" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="O181" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="182" spans="1:15" x14ac:dyDescent="0.25">
@@ -7942,7 +9585,7 @@
         <v>342</v>
       </c>
       <c r="I182" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="183" spans="1:15" x14ac:dyDescent="0.25">
@@ -8028,13 +9671,13 @@
         <v>342</v>
       </c>
       <c r="I185" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="M185" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O185" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="186" spans="1:15" x14ac:dyDescent="0.25">
@@ -8090,10 +9733,10 @@
         <v>2582580623</v>
       </c>
       <c r="I187" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="M187" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="188" spans="1:15" x14ac:dyDescent="0.25">
@@ -8122,13 +9765,13 @@
         <v>2582580620</v>
       </c>
       <c r="I188" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="M188" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="O188" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="189" spans="1:15" x14ac:dyDescent="0.25">
@@ -8157,13 +9800,13 @@
         <v>2582580615</v>
       </c>
       <c r="I189" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="M189" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="O189" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="190" spans="1:15" x14ac:dyDescent="0.25">
@@ -8192,13 +9835,13 @@
         <v>342</v>
       </c>
       <c r="I190" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="M190" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="O190" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="191" spans="1:15" x14ac:dyDescent="0.25">
@@ -8227,7 +9870,7 @@
         <v>2593339189</v>
       </c>
       <c r="I191" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="192" spans="1:15" x14ac:dyDescent="0.25">
@@ -8283,10 +9926,10 @@
         <v>342</v>
       </c>
       <c r="I193" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M193" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="194" spans="1:15" x14ac:dyDescent="0.25">
@@ -8315,13 +9958,13 @@
         <v>2582580625</v>
       </c>
       <c r="I194" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="M194" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="O194" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="195" spans="1:15" x14ac:dyDescent="0.25">
@@ -8406,10 +10049,10 @@
         <v>342</v>
       </c>
       <c r="I197" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="O197" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="198" spans="1:15" x14ac:dyDescent="0.25">
@@ -8439,7 +10082,7 @@
       </c>
       <c r="I198" s="1"/>
       <c r="O198" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="199" spans="1:15" x14ac:dyDescent="0.25">
@@ -8468,7 +10111,7 @@
         <v>2593339181</v>
       </c>
       <c r="I199" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="200" spans="1:15" x14ac:dyDescent="0.25">
@@ -8524,10 +10167,10 @@
         <v>2582580639</v>
       </c>
       <c r="I201" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="O201" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="202" spans="1:15" x14ac:dyDescent="0.25">
@@ -8556,10 +10199,10 @@
         <v>342</v>
       </c>
       <c r="I202" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="M202" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="203" spans="1:15" x14ac:dyDescent="0.25">
@@ -8588,7 +10231,7 @@
         <v>342</v>
       </c>
       <c r="I203" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="204" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added 10 more IMG annotations of genomes
</commit_message>
<xml_diff>
--- a/Data_files/combined_genome_data.xlsx
+++ b/Data_files/combined_genome_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\MAGstravaganza\Data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amlin\Desktop\MAGstravaganza\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="751">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="778">
   <si>
     <t>ME</t>
   </si>
@@ -2277,12 +2277,93 @@
   </si>
   <si>
     <t>glycolate, trehalose, maltose, cellobiose, glucose</t>
+  </si>
+  <si>
+    <t>heme, LPS export, lipoprotein release, oligopepteide, phosphate, phospholipid, phosphonate, spermidine/putrescine</t>
+  </si>
+  <si>
+    <t>flagellum with type III secretion</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose, fructose, galactose, mannose, sucrose, galacturonate, maltose</t>
+  </si>
+  <si>
+    <t>some carotenoid synthesis</t>
+  </si>
+  <si>
+    <t>chitobiose, glycolate, cellobiose, glucose</t>
+  </si>
+  <si>
+    <t>heme, iron, LPS export, lipoprotein release, peptide/nickel, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>glycolate, cellobiose</t>
+  </si>
+  <si>
+    <t>methionine, arginine/lysine/histidine/glutamine, bicarbonate, biotin, branched amino, carbohydrate, cobalt/nickel, L-amino acid, iron, LPS export, LPS transport, molybdate, neutral amino, nitrate/nitrite, phosphate, phospholipid/cholesterol, phosphonate, chitobiose, spermidine/putrescine, sulfate, urea</t>
+  </si>
+  <si>
+    <t>nitrate_red_ass, nitrogen fixation, ammonia_assimilation</t>
+  </si>
+  <si>
+    <t>carbon fixation (Rubisco), chitobiose, glucose, glycolate, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>heme, LPS export, lipoprotein, molybdate, oligopeptide, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>glucose, galactose, cellulose degradation, maltose, starch/glycogen</t>
+  </si>
+  <si>
+    <t>iron, LPS export, LPS transport, lipoprotein release, peptide/nickel, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>LPS export, lipoprotein release, phosphate, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>one sulfate_red_ass gene</t>
+  </si>
+  <si>
+    <t>cellulose degradation</t>
+  </si>
+  <si>
+    <t>polysaccharide phosphate, heme, LPS export, LPS transport, lipoprotein release, phosphate, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>chitin degradation, glycolate, cellulose degradation</t>
+  </si>
+  <si>
+    <t>heme, iron (III), LPS export, lipoprotein release, phosphate, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>alkanesulfonate</t>
+  </si>
+  <si>
+    <t>Oxidative phosphorylation, luciferase gene?</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose, galactose, fructose, starch/glycogen, cellulose degradation, maltose</t>
+  </si>
+  <si>
+    <t>iron, LPS export, peptide/nickel, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>galactose, melibiose, cellobiose</t>
+  </si>
+  <si>
+    <t>branched amino, carbohydrate, LPS export, oligopeptide, peptide/nickel, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, one nitritre reductase</t>
+  </si>
+  <si>
+    <t>glucose, galacturonate, cellobiose, starch/glycogen, maltose</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2681,8 +2762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I37" workbookViewId="0">
-      <selection activeCell="L69" sqref="L69"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="L80" sqref="L80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6049,8 +6130,29 @@
       <c r="I70" s="1" t="s">
         <v>496</v>
       </c>
+      <c r="J70" t="s">
+        <v>753</v>
+      </c>
       <c r="K70" t="s">
         <v>345</v>
+      </c>
+      <c r="L70" t="s">
+        <v>661</v>
+      </c>
+      <c r="N70" t="s">
+        <v>461</v>
+      </c>
+      <c r="P70" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>751</v>
+      </c>
+      <c r="S70" t="s">
+        <v>752</v>
+      </c>
+      <c r="T70" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
@@ -6081,6 +6183,21 @@
       <c r="I71" s="1" t="s">
         <v>367</v>
       </c>
+      <c r="J71" t="s">
+        <v>755</v>
+      </c>
+      <c r="L71" t="s">
+        <v>754</v>
+      </c>
+      <c r="N71" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>586</v>
+      </c>
+      <c r="T71" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
@@ -6110,6 +6227,21 @@
       <c r="I72" s="1" t="s">
         <v>431</v>
       </c>
+      <c r="K72" t="s">
+        <v>757</v>
+      </c>
+      <c r="L72" t="s">
+        <v>701</v>
+      </c>
+      <c r="N72" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>756</v>
+      </c>
+      <c r="T72" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
@@ -6139,8 +6271,23 @@
       <c r="I73" s="1" t="s">
         <v>377</v>
       </c>
+      <c r="J73" t="s">
+        <v>760</v>
+      </c>
+      <c r="L73" t="s">
+        <v>754</v>
+      </c>
       <c r="M73" t="s">
         <v>479</v>
+      </c>
+      <c r="N73" t="s">
+        <v>759</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>758</v>
+      </c>
+      <c r="T73" t="s">
+        <v>603</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
@@ -6171,8 +6318,26 @@
       <c r="I74" s="1" t="s">
         <v>378</v>
       </c>
+      <c r="J74" t="s">
+        <v>701</v>
+      </c>
+      <c r="L74" t="s">
+        <v>762</v>
+      </c>
       <c r="M74" t="s">
         <v>474</v>
+      </c>
+      <c r="N74" t="s">
+        <v>461</v>
+      </c>
+      <c r="P74" t="s">
+        <v>634</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>761</v>
+      </c>
+      <c r="T74" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
@@ -6203,8 +6368,20 @@
       <c r="I75" s="1" t="s">
         <v>376</v>
       </c>
+      <c r="J75" t="s">
+        <v>611</v>
+      </c>
       <c r="M75" t="s">
         <v>469</v>
+      </c>
+      <c r="N75" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>763</v>
+      </c>
+      <c r="T75" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.25">
@@ -6233,6 +6410,24 @@
         <v>342</v>
       </c>
       <c r="I76" s="1"/>
+      <c r="J76" t="s">
+        <v>701</v>
+      </c>
+      <c r="L76" t="s">
+        <v>766</v>
+      </c>
+      <c r="N76" t="s">
+        <v>461</v>
+      </c>
+      <c r="P76" t="s">
+        <v>765</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>764</v>
+      </c>
+      <c r="T76" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
@@ -6262,6 +6457,21 @@
       <c r="I77" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="J77" t="s">
+        <v>701</v>
+      </c>
+      <c r="L77" t="s">
+        <v>768</v>
+      </c>
+      <c r="N77" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>767</v>
+      </c>
+      <c r="T77" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
@@ -6291,8 +6501,29 @@
       <c r="I78" s="1" t="s">
         <v>379</v>
       </c>
+      <c r="J78" t="s">
+        <v>723</v>
+      </c>
+      <c r="L78" t="s">
+        <v>772</v>
+      </c>
       <c r="M78" t="s">
         <v>475</v>
+      </c>
+      <c r="N78" t="s">
+        <v>461</v>
+      </c>
+      <c r="P78" t="s">
+        <v>770</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>769</v>
+      </c>
+      <c r="S78" t="s">
+        <v>604</v>
+      </c>
+      <c r="T78" t="s">
+        <v>771</v>
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
@@ -6323,6 +6554,18 @@
       <c r="I79" s="1" t="s">
         <v>382</v>
       </c>
+      <c r="J79" t="s">
+        <v>701</v>
+      </c>
+      <c r="L79" t="s">
+        <v>774</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>773</v>
+      </c>
+      <c r="T79" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
@@ -6351,6 +6594,27 @@
       </c>
       <c r="I80" s="1" t="s">
         <v>352</v>
+      </c>
+      <c r="J80" t="s">
+        <v>701</v>
+      </c>
+      <c r="L80" t="s">
+        <v>777</v>
+      </c>
+      <c r="N80" t="s">
+        <v>776</v>
+      </c>
+      <c r="P80" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>775</v>
+      </c>
+      <c r="S80" t="s">
+        <v>752</v>
+      </c>
+      <c r="T80" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added a couple more genomes
</commit_message>
<xml_diff>
--- a/Data_files/combined_genome_data.xlsx
+++ b/Data_files/combined_genome_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1791" uniqueCount="783">
   <si>
     <t>ME</t>
   </si>
@@ -2358,6 +2358,21 @@
   </si>
   <si>
     <t>glucose, galacturonate, cellobiose, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>iron, LPS export, LPS transport, lipoprotein release, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>galactose, lactose, sucrose, glycolate, cellobiose, starch/glycogen, galacturonate</t>
+  </si>
+  <si>
+    <t>branched amino, iron (III), LPS export, manganese/zinc/iron, microcin C, molybdate, monosaccharide, oligopeptide, peptide/nickel, phosphate, phospholipid/cholesterol, spermidine/putrescine, xylose, zinc</t>
+  </si>
+  <si>
+    <t>partial sulfate_red_ass, alkanesulfonate</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose, galactose, melibiose, glycolate, cellobiose, starch/glycogen, maltose, galacturonate</t>
   </si>
 </sst>
 </file>
@@ -2762,8 +2777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="L80" sqref="L80"/>
+    <sheetView tabSelected="1" topLeftCell="J65" workbookViewId="0">
+      <selection activeCell="L82" sqref="L82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6617,7 +6632,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>2582580592</v>
       </c>
@@ -6645,8 +6660,26 @@
       <c r="I81" s="1" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J81" t="s">
+        <v>723</v>
+      </c>
+      <c r="L81" t="s">
+        <v>779</v>
+      </c>
+      <c r="N81" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>778</v>
+      </c>
+      <c r="S81" t="s">
+        <v>604</v>
+      </c>
+      <c r="T81" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>2582580593</v>
       </c>
@@ -6674,11 +6707,26 @@
       <c r="I82" s="1" t="s">
         <v>380</v>
       </c>
+      <c r="L82" t="s">
+        <v>782</v>
+      </c>
+      <c r="N82" t="s">
+        <v>461</v>
+      </c>
       <c r="O82" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P82" t="s">
+        <v>781</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>780</v>
+      </c>
+      <c r="T82" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>2582580594</v>
       </c>
@@ -6705,7 +6753,7 @@
       </c>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>2582580595</v>
       </c>
@@ -6737,7 +6785,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>2582580596</v>
       </c>
@@ -6769,7 +6817,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>2582580597</v>
       </c>
@@ -6798,7 +6846,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>2582580598</v>
       </c>
@@ -6827,7 +6875,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>2582580599</v>
       </c>
@@ -6859,7 +6907,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>2582580600</v>
       </c>
@@ -6897,7 +6945,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>2582580601</v>
       </c>
@@ -6932,7 +6980,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>2582580602</v>
       </c>
@@ -6961,7 +7009,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>2582580603</v>
       </c>
@@ -6996,7 +7044,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>2582580604</v>
       </c>
@@ -7023,7 +7071,7 @@
       </c>
       <c r="I93" s="1"/>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>2582580605</v>
       </c>
@@ -7055,7 +7103,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>2582580606</v>
       </c>
@@ -7090,7 +7138,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>2582580607</v>
       </c>

</xml_diff>

<commit_message>
Up to 92 genomes done
</commit_message>
<xml_diff>
--- a/Data_files/combined_genome_data.xlsx
+++ b/Data_files/combined_genome_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1817" uniqueCount="796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1848" uniqueCount="815">
   <si>
     <t>ME</t>
   </si>
@@ -2412,6 +2412,63 @@
   </si>
   <si>
     <t>UDP-NAG</t>
+  </si>
+  <si>
+    <t>heme, iron, LPS export, lipoprotein release, peptide/nickel, phosphate, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>chitobiose</t>
+  </si>
+  <si>
+    <t>glutamate, amino acid/amide, branched aminos, iron, iron (III), LPS export, lipoprotein release, maltose/maltodextrin, molybdate, nitrate/nitrite, oligopeptide, osmoprotectant, phospholipid/cholesterol, phosphonate, sorbitol, sulfate, tungstate, some type II secretion, lots of general secretion</t>
+  </si>
+  <si>
+    <t>carotenoid biosynthesis, carbon fixation via Rubisco, formate</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, nitronate monooxygenase, nitrate transporter but no reduction</t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, sulfide_ox, methane_sulfonate, alkane_sulfonate</t>
+  </si>
+  <si>
+    <t>flagellum</t>
+  </si>
+  <si>
+    <t>chitobiose, MurNAc/UDP-NAG, fructose, glucose, galactose, glycolate, starch/glycogen, trehalose, maltose</t>
+  </si>
+  <si>
+    <t>heme, iron(III), LPS export, lipoprotein release, phospholipid/cholesterol, phosphate, molybdate</t>
+  </si>
+  <si>
+    <t>three carotenoid genes, Wood-Ljungdahl, formate</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose, galactose, fructan, rhamnulose, cellulose, glucoside, cellobiose, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>iron, LPS export, lipoprotein release, phospholipid/cholesterol, sodium</t>
+  </si>
+  <si>
+    <t>two carotenoid genes, formate</t>
+  </si>
+  <si>
+    <t>fructose, cellobiose, glucoside,  maltose, sucrose</t>
+  </si>
+  <si>
+    <t>heme, iron, LPS export, lipoprotein release, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, one nitrate reductase, nitroalkane monooxygenase</t>
+  </si>
+  <si>
+    <t>three carotenoid genes, formate</t>
+  </si>
+  <si>
+    <t>some chemotaxis</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose, galactose, fructan, sucrose, glycolate, glucoside, cellobiose, maltose, isomaltose, dextrin, UDP-galacturonate, starch/glycogen</t>
   </si>
 </sst>
 </file>
@@ -2816,8 +2873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" topLeftCell="H76" workbookViewId="0">
+      <selection activeCell="L92" sqref="L92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7020,8 +7077,29 @@
       <c r="I88" s="1" t="s">
         <v>376</v>
       </c>
+      <c r="J88" t="s">
+        <v>723</v>
+      </c>
+      <c r="L88" t="s">
+        <v>797</v>
+      </c>
       <c r="M88" t="s">
         <v>469</v>
+      </c>
+      <c r="N88" t="s">
+        <v>461</v>
+      </c>
+      <c r="P88" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>796</v>
+      </c>
+      <c r="S88" t="s">
+        <v>604</v>
+      </c>
+      <c r="T88" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.25">
@@ -7052,14 +7130,35 @@
       <c r="I89" s="1" t="s">
         <v>457</v>
       </c>
+      <c r="J89" t="s">
+        <v>799</v>
+      </c>
       <c r="K89" t="s">
         <v>383</v>
       </c>
+      <c r="L89" t="s">
+        <v>803</v>
+      </c>
       <c r="M89" t="s">
         <v>480</v>
       </c>
+      <c r="N89" t="s">
+        <v>800</v>
+      </c>
       <c r="O89" t="s">
         <v>501</v>
+      </c>
+      <c r="P89" t="s">
+        <v>801</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>798</v>
+      </c>
+      <c r="S89" t="s">
+        <v>802</v>
+      </c>
+      <c r="T89" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.25">
@@ -7090,11 +7189,26 @@
       <c r="I90" s="1" t="s">
         <v>384</v>
       </c>
+      <c r="J90" t="s">
+        <v>805</v>
+      </c>
+      <c r="L90" t="s">
+        <v>806</v>
+      </c>
       <c r="M90" t="s">
         <v>481</v>
       </c>
+      <c r="N90" t="s">
+        <v>461</v>
+      </c>
       <c r="O90" t="s">
         <v>502</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>804</v>
+      </c>
+      <c r="T90" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.25">
@@ -7125,6 +7239,24 @@
       <c r="I91" s="1" t="s">
         <v>385</v>
       </c>
+      <c r="J91" t="s">
+        <v>808</v>
+      </c>
+      <c r="L91" t="s">
+        <v>809</v>
+      </c>
+      <c r="P91" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>807</v>
+      </c>
+      <c r="S91" t="s">
+        <v>604</v>
+      </c>
+      <c r="T91" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
@@ -7154,11 +7286,29 @@
       <c r="I92" s="1" t="s">
         <v>386</v>
       </c>
+      <c r="J92" t="s">
+        <v>812</v>
+      </c>
+      <c r="L92" t="s">
+        <v>814</v>
+      </c>
       <c r="M92" t="s">
         <v>458</v>
       </c>
+      <c r="N92" t="s">
+        <v>811</v>
+      </c>
       <c r="O92" t="s">
         <v>502</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>810</v>
+      </c>
+      <c r="S92" t="s">
+        <v>813</v>
+      </c>
+      <c r="T92" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Made it to the Trout Bog genomes!
</commit_message>
<xml_diff>
--- a/Data_files/combined_genome_data.xlsx
+++ b/Data_files/combined_genome_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1848" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1953" uniqueCount="866">
   <si>
     <t>ME</t>
   </si>
@@ -2469,6 +2469,159 @@
   </si>
   <si>
     <t>chitobiose, glucose, galactose, fructan, sucrose, glycolate, glucoside, cellobiose, maltose, isomaltose, dextrin, UDP-galacturonate, starch/glycogen</t>
+  </si>
+  <si>
+    <t>branched amino, carbohydrate, LPS export, lipoprotein release, manganese/zinc/iron, molybdate, monosaccharide, oligopeptide, ribose, some type VI secretion</t>
+  </si>
+  <si>
+    <t>fructose, galactose, galactonate, trehalose, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>heme, iron(III), LPS export, lipoprotein release, phosphate, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>chitobiose, glycolate</t>
+  </si>
+  <si>
+    <t>amino acid/amide, branched amino, iron, LPS export, lipoprotein, oligopeptide, phosphate, phospholipid/cholesterol, lipoprotein release, oligopepetide, phosphate, ribose, sodium, urea</t>
+  </si>
+  <si>
+    <t>MurNAc, galactose, rhamnulose, cellulose, starch/glycogen, trehalose</t>
+  </si>
+  <si>
+    <t>zinc, amino acid/amide, carbohydrate, iron, iron (III), LPS export, lipoprotein release, manganese/iron, molybdate, monosaccharide, oligopeptide, peptide/nickel, phosphate, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>chitin, chitobiose, MurNAc, glucose, rhamnulose, galactose, glycolate, glycerate, cellulose, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>xylose, alpha-glucoside, branched amino, carbohydrate, cobalt/nickel, iron, iron(III), monosaccharide, multiple sugar, phosphate, raffinose/stachyose/melibiose, spermidine/putrescine</t>
+  </si>
+  <si>
+    <t>glucose, alpha-galactosidase, glycolate, maltose, starch/glycogen</t>
+  </si>
+  <si>
+    <t>cobalt/nickel, iron, iron(III), LPS export, lipoprotein release, microcin C, molybdate, oligopeptide, phosphate, phospholipid/cholesterol, putrescine</t>
+  </si>
+  <si>
+    <t>chemotaxis, flagellum</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose, starch/glycogen</t>
+  </si>
+  <si>
+    <t>heme, LPS export, lipoprotein release, peptide/nickel, phosphate, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>chitobiose, cellulose</t>
+  </si>
+  <si>
+    <t>iron, iron(III), LPS export, lipoprotein, lipoprotein release, manganese/zinc, monosaccharide, phosphate, phospholipid/cholesterol, ribose, sulfate, urea-binding protein</t>
+  </si>
+  <si>
+    <t>chemotaxis (monosaccharide, purine, ribose?), some flagellum proteins</t>
+  </si>
+  <si>
+    <t>fructose, glucose, rhamnulose, alpha galactosidase, cellulose, cellobiose, trehalose, starch/glycogen, galacturonate</t>
+  </si>
+  <si>
+    <t>chitobiose, glycolate, maltose</t>
+  </si>
+  <si>
+    <t>heme, iron(III), LPS export, lipoprotein release, molybdate, phosphate, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>chitobiose, fructose, rhamnulose, galactose, cellulose degradation, cellobiose, glucoside, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>heme, LPS export, lipoprotein release, molybdate, nitrate/nitrite, phosphate, phospholipid/cholesterol, sulfate, sulfonate, urea</t>
+  </si>
+  <si>
+    <t>partial nitrate_red_dis, hydroxylamine synthesis, nitrile, ammonia_assimilation</t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, alkanesulfonate, methanesulfonate</t>
+  </si>
+  <si>
+    <t>chemotaxis (purine?), flagellum</t>
+  </si>
+  <si>
+    <t>methane, methanol, formate, glucose, galacturonate, glucoside, cellobiose, starch/glycogen, maltose, trehalose</t>
+  </si>
+  <si>
+    <t>amino acid/amide, extracellular solute, inositol, iron, iron(III), LPS export, lipoprotein, microcin C, oligopeptide, peptide/nickel, phosphate, phospholipid/cholesterol, xylitol, urea, zinc</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose, rhamnulose, glycolate, cellulose, starch/glycogen, maltose, pectin</t>
+  </si>
+  <si>
+    <t>branched amino, amino acid/amide, biotin, iron, phosphate, polar amino</t>
+  </si>
+  <si>
+    <t>partial sufate_red_ass</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose, glucoside, cellobiose</t>
+  </si>
+  <si>
+    <t>LPS export, amino acid/amide, branched amino, microcin C, molybdate, nitrate/nitrite, paraquat-inducible protein, phosphate, phospholipid/cholesterol, tungstate</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, nitroalkane, one nitrate_red_ass, one nitrate_red_dis, nitrile</t>
+  </si>
+  <si>
+    <t>Wood-Ljungdahl, formate, formaldehyde(?), glycolate</t>
+  </si>
+  <si>
+    <t>dipthamide, amino acid/amide, branched amino, heme, iron, LPS export, lipoprotein release, molybdate, molbdenum, nitrate/nitrite, phosphate, phospholipid/cholesterol, sulfate, sulfonate, tungstate, urea</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, nitroalkane, transporters for nitrate but no reduction</t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, sulfur_oxidation (SOX), taurine, alkanesulfonate, methansulfonate</t>
+  </si>
+  <si>
+    <t>formate, glycolate, chitobiose, MurNAc,</t>
+  </si>
+  <si>
+    <t>amino acid/amide, cobalt/nickel, iron, LPS export, lipopolysaccharide, macrolide, manganese/zinc/iron, molybdate, phosphate, phospholipid/cholesterol, sulfate, sulfonate, thiol reductant</t>
+  </si>
+  <si>
+    <t>carotenoid synthesis, reductive TCA</t>
+  </si>
+  <si>
+    <t>nitrogen_fixation, ammonia_assimilation</t>
+  </si>
+  <si>
+    <t>chitobiose, MurNAc, glucose</t>
+  </si>
+  <si>
+    <t>LPS export, lipoprotein release, molybdate, oligopeptide, phosphate, phospholipid/cholesterol, sulfate</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, nitrile</t>
+  </si>
+  <si>
+    <t>partial sulfate_red_ass, partial sulfur_oxidation (SOX)</t>
+  </si>
+  <si>
+    <t>methanol, formaldehyde, formate, chitobiose, glucose, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>LPS export, lipoprotein release, oligopeptide, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>amino acid/amide, capsular polysaccharide, cobalt/nickel, iron, LPS export, lipoprotein release, macrolide, manganese/zinc/iron, molybdate, phosphate, phospholipid/cholesterol, sulfate, sulfonate, type IV secretion</t>
+  </si>
+  <si>
+    <t>reductive TCA</t>
+  </si>
+  <si>
+    <t>nitrogen_fixation, ammonia_assimilation, hydroxylamine reductase</t>
+  </si>
+  <si>
+    <t>carotenoid synthesis, chitobiose, glucose, starch/glycogen, dextrin, maltose</t>
   </si>
 </sst>
 </file>
@@ -2873,8 +3026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H76" workbookViewId="0">
-      <selection activeCell="L92" sqref="L92"/>
+    <sheetView tabSelected="1" topLeftCell="G111" workbookViewId="0">
+      <selection activeCell="J113" sqref="J113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7337,6 +7490,18 @@
         <v>342</v>
       </c>
       <c r="I93" s="1"/>
+      <c r="L93" t="s">
+        <v>816</v>
+      </c>
+      <c r="N93" t="s">
+        <v>694</v>
+      </c>
+      <c r="P93" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>815</v>
+      </c>
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
@@ -7366,8 +7531,20 @@
       <c r="I94" s="1" t="s">
         <v>356</v>
       </c>
+      <c r="L94" t="s">
+        <v>818</v>
+      </c>
       <c r="M94" t="s">
         <v>469</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>817</v>
+      </c>
+      <c r="S94" t="s">
+        <v>604</v>
+      </c>
+      <c r="T94" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.25">
@@ -7398,11 +7575,32 @@
       <c r="I95" s="1" t="s">
         <v>386</v>
       </c>
+      <c r="J95" t="s">
+        <v>419</v>
+      </c>
+      <c r="L95" t="s">
+        <v>820</v>
+      </c>
       <c r="M95" t="s">
         <v>469</v>
       </c>
+      <c r="N95" t="s">
+        <v>694</v>
+      </c>
       <c r="O95" t="s">
         <v>502</v>
+      </c>
+      <c r="P95" t="s">
+        <v>653</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>819</v>
+      </c>
+      <c r="S95" t="s">
+        <v>594</v>
+      </c>
+      <c r="T95" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.25">
@@ -7433,14 +7631,29 @@
       <c r="I96" s="1" t="s">
         <v>433</v>
       </c>
+      <c r="L96" t="s">
+        <v>822</v>
+      </c>
       <c r="M96" t="s">
         <v>482</v>
       </c>
+      <c r="N96" t="s">
+        <v>461</v>
+      </c>
       <c r="O96" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P96" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>821</v>
+      </c>
+      <c r="T96" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>2582580608</v>
       </c>
@@ -7468,8 +7681,23 @@
       <c r="I97" s="1" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J97" t="s">
+        <v>701</v>
+      </c>
+      <c r="L97" t="s">
+        <v>824</v>
+      </c>
+      <c r="N97" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>823</v>
+      </c>
+      <c r="T97" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>2582580609</v>
       </c>
@@ -7497,8 +7725,29 @@
       <c r="I98" s="1" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J98" t="s">
+        <v>808</v>
+      </c>
+      <c r="L98" t="s">
+        <v>827</v>
+      </c>
+      <c r="N98" t="s">
+        <v>461</v>
+      </c>
+      <c r="O98" t="s">
+        <v>616</v>
+      </c>
+      <c r="P98" t="s">
+        <v>826</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>825</v>
+      </c>
+      <c r="T98" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>2582580610</v>
       </c>
@@ -7524,8 +7773,26 @@
         <v>342</v>
       </c>
       <c r="I99" s="1"/>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J99" t="s">
+        <v>723</v>
+      </c>
+      <c r="L99" t="s">
+        <v>829</v>
+      </c>
+      <c r="N99" t="s">
+        <v>791</v>
+      </c>
+      <c r="O99" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>828</v>
+      </c>
+      <c r="T99" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>2582580611</v>
       </c>
@@ -7556,11 +7823,23 @@
       <c r="M100" t="s">
         <v>471</v>
       </c>
+      <c r="N100" t="s">
+        <v>461</v>
+      </c>
       <c r="O100" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P100" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>830</v>
+      </c>
+      <c r="T100" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>2582580612</v>
       </c>
@@ -7586,14 +7865,23 @@
         <v>342</v>
       </c>
       <c r="I101" s="1"/>
+      <c r="J101" t="s">
+        <v>832</v>
+      </c>
       <c r="M101" t="s">
         <v>458</v>
       </c>
       <c r="O101" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P101" t="s">
+        <v>831</v>
+      </c>
+      <c r="T101" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>2582580613</v>
       </c>
@@ -7621,14 +7909,26 @@
       <c r="I102" s="1" t="s">
         <v>435</v>
       </c>
+      <c r="J102" t="s">
+        <v>701</v>
+      </c>
+      <c r="L102" t="s">
+        <v>833</v>
+      </c>
       <c r="M102" t="s">
         <v>469</v>
       </c>
       <c r="O102" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q102" t="s">
+        <v>657</v>
+      </c>
+      <c r="T102" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>2582580614</v>
       </c>
@@ -7656,11 +7956,29 @@
       <c r="I103" s="1" t="s">
         <v>356</v>
       </c>
+      <c r="J103" t="s">
+        <v>723</v>
+      </c>
+      <c r="L103" t="s">
+        <v>835</v>
+      </c>
+      <c r="N103" t="s">
+        <v>461</v>
+      </c>
       <c r="O103" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q103" t="s">
+        <v>834</v>
+      </c>
+      <c r="S103" t="s">
+        <v>604</v>
+      </c>
+      <c r="T103" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>2582580615</v>
       </c>
@@ -7688,14 +8006,32 @@
       <c r="I104" s="1" t="s">
         <v>436</v>
       </c>
+      <c r="J104" t="s">
+        <v>840</v>
+      </c>
       <c r="M104" t="s">
         <v>470</v>
       </c>
+      <c r="N104" t="s">
+        <v>837</v>
+      </c>
       <c r="O104" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P104" t="s">
+        <v>838</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>836</v>
+      </c>
+      <c r="S104" t="s">
+        <v>839</v>
+      </c>
+      <c r="T104" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>2582580616</v>
       </c>
@@ -7721,11 +8057,26 @@
         <v>342</v>
       </c>
       <c r="I105" s="1"/>
+      <c r="J105" t="s">
+        <v>842</v>
+      </c>
       <c r="M105" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N105" t="s">
+        <v>461</v>
+      </c>
+      <c r="P105" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>841</v>
+      </c>
+      <c r="T105" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>2582580617</v>
       </c>
@@ -7751,8 +8102,20 @@
         <v>2582580671</v>
       </c>
       <c r="I106" s="1"/>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N106" t="s">
+        <v>461</v>
+      </c>
+      <c r="P106" t="s">
+        <v>844</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>843</v>
+      </c>
+      <c r="T106" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>2582580620</v>
       </c>
@@ -7780,14 +8143,32 @@
       <c r="I107" s="1" t="s">
         <v>437</v>
       </c>
+      <c r="J107" t="s">
+        <v>845</v>
+      </c>
+      <c r="K107" t="s">
+        <v>848</v>
+      </c>
       <c r="M107" t="s">
         <v>484</v>
       </c>
+      <c r="N107" t="s">
+        <v>847</v>
+      </c>
       <c r="O107" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P107" t="s">
+        <v>530</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>846</v>
+      </c>
+      <c r="T107" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>2582580621</v>
       </c>
@@ -7815,14 +8196,32 @@
       <c r="I108" s="1" t="s">
         <v>356</v>
       </c>
+      <c r="J108" t="s">
+        <v>852</v>
+      </c>
       <c r="K108" t="s">
         <v>389</v>
       </c>
+      <c r="N108" t="s">
+        <v>850</v>
+      </c>
       <c r="O108" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P108" t="s">
+        <v>851</v>
+      </c>
+      <c r="Q108" t="s">
+        <v>849</v>
+      </c>
+      <c r="S108" t="s">
+        <v>622</v>
+      </c>
+      <c r="T108" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>2582580622</v>
       </c>
@@ -7850,14 +8249,35 @@
       <c r="I109" s="1" t="s">
         <v>453</v>
       </c>
+      <c r="J109" t="s">
+        <v>854</v>
+      </c>
+      <c r="L109" t="s">
+        <v>856</v>
+      </c>
       <c r="M109" t="s">
         <v>485</v>
       </c>
+      <c r="N109" t="s">
+        <v>855</v>
+      </c>
       <c r="O109" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P109" t="s">
+        <v>634</v>
+      </c>
+      <c r="Q109" t="s">
+        <v>853</v>
+      </c>
+      <c r="S109" t="s">
+        <v>604</v>
+      </c>
+      <c r="T109" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>2582580623</v>
       </c>
@@ -7885,11 +8305,26 @@
       <c r="I110" s="1" t="s">
         <v>390</v>
       </c>
+      <c r="J110" t="s">
+        <v>860</v>
+      </c>
       <c r="M110" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N110" t="s">
+        <v>858</v>
+      </c>
+      <c r="P110" t="s">
+        <v>859</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>857</v>
+      </c>
+      <c r="T110" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>2582580624</v>
       </c>
@@ -7915,11 +8350,26 @@
         <v>2582580699</v>
       </c>
       <c r="I111" s="1"/>
+      <c r="J111" t="s">
+        <v>797</v>
+      </c>
       <c r="M111" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N111" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q111" t="s">
+        <v>861</v>
+      </c>
+      <c r="S111" t="s">
+        <v>826</v>
+      </c>
+      <c r="T111" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>2582580625</v>
       </c>
@@ -7945,14 +8395,29 @@
         <v>2593339184</v>
       </c>
       <c r="I112" s="1"/>
+      <c r="J112" t="s">
+        <v>865</v>
+      </c>
+      <c r="L112" t="s">
+        <v>863</v>
+      </c>
       <c r="M112" t="s">
         <v>486</v>
       </c>
+      <c r="N112" t="s">
+        <v>864</v>
+      </c>
       <c r="O112" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q112" t="s">
+        <v>862</v>
+      </c>
+      <c r="T112" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>2582580627</v>
       </c>
@@ -7986,8 +8451,11 @@
       <c r="O113" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P113" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>2582580628</v>
       </c>
@@ -8016,7 +8484,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>2582580629</v>
       </c>
@@ -8046,7 +8514,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>2582580630</v>
       </c>
@@ -8078,7 +8546,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>2582580631</v>
       </c>
@@ -8107,7 +8575,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>2582580632</v>
       </c>
@@ -8136,7 +8604,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>2582580633</v>
       </c>
@@ -8166,7 +8634,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>2582580634</v>
       </c>
@@ -8195,7 +8663,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>2582580635</v>
       </c>
@@ -8224,7 +8692,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>2582580637</v>
       </c>
@@ -8256,7 +8724,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>2582580638</v>
       </c>
@@ -8291,7 +8759,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>2582580639</v>
       </c>
@@ -8323,7 +8791,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>2582580640</v>
       </c>
@@ -8358,7 +8826,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>2582580641</v>
       </c>
@@ -8390,7 +8858,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>2582580642</v>
       </c>
@@ -8423,7 +8891,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>2582580643</v>
       </c>

</xml_diff>

<commit_message>
I think I forgot to commit this last time
</commit_message>
<xml_diff>
--- a/Data_files/combined_genome_data.xlsx
+++ b/Data_files/combined_genome_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2057" uniqueCount="916">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2108" uniqueCount="949">
   <si>
     <t>ME</t>
   </si>
@@ -2772,6 +2772,105 @@
   </si>
   <si>
     <t>formate, chitobiose, glycolate</t>
+  </si>
+  <si>
+    <t>branched amino, amino acid/amide, iron, LPS export, molybdate, oligopeptide/dipeptide, phosphate, phospholipid/cholesterol, sodium, tungstate/molybdate</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, nitrogen_fixation, nitrous oxide reductase, one nitrate reductase</t>
+  </si>
+  <si>
+    <t>thiosulfate, one sulfite reductase, no evidence for sulfate oxidation</t>
+  </si>
+  <si>
+    <t>MurNAc, chitobiose, glucose, glycolate, starch/glycogen</t>
+  </si>
+  <si>
+    <t>LPS export, phosphate, lipoprotein-release, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>nitrilase</t>
+  </si>
+  <si>
+    <t>methanol, formate</t>
+  </si>
+  <si>
+    <t>partial sulfur oxidation</t>
+  </si>
+  <si>
+    <t>MurNAc, chitobiose, fructose</t>
+  </si>
+  <si>
+    <t>glutamate, amino acid/amide, glutamate/aspartate, heme, phosphate, phospholipid</t>
+  </si>
+  <si>
+    <t>MurNAc, chitobiose, fructose, glycolate, galacturonate</t>
+  </si>
+  <si>
+    <t>amino acid/amide, branched amino, cobalt/nickel, iron, LPS export, lipoprotein release, macrolide, molybdate, manganese/zinc/iron, phosphate, sulfate, sulfonate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carotenoid synthesis, carbon fixation (RuBisCo), carbon fixation (reductive TCA), </t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, nitrogen fixation</t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, alkane_sulfonate</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose, starch/glycogen, galacturonate</t>
+  </si>
+  <si>
+    <t>one type IV gene</t>
+  </si>
+  <si>
+    <t>can make dextrin?</t>
+  </si>
+  <si>
+    <t>branched amino (lots), glutamate, amino acid/amide (lots), carbohydrate, dipeptide, glutathione, heme, iron, iron(III), LPS export, lipoprotein release, molybdate, monosaccharide, oligopeptide, phospholipid/cholesterol, phosphonate, putrescine, ribose, spermidine/putrescine, sulfate, tungstate, urea</t>
+  </si>
+  <si>
+    <t>Wood-Ljungdahl, formate</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, partial denitrification, partial nitrification, nitrate/nitrite transporter</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose, glyceraldehyde, starch/glycogen, galacturonate</t>
+  </si>
+  <si>
+    <t>LPS export, molybdate, phosphate, phospholipid/cholesterol, zinc</t>
+  </si>
+  <si>
+    <t>ammonia_assimlation, nitrate_red_ass, 3/4 denitrification, nitrogen fixation, partial nitrate_red_ass</t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, sulfate oxidation (SOX), thiosulfate</t>
+  </si>
+  <si>
+    <t>carbon fixation (reductive TCA), formate, glucose, NAG, glycolate, starch/glycogen</t>
+  </si>
+  <si>
+    <t>ribose, xylose, amino acid/amide, biotin, branched amino, carbohydrate, iron, monosaccharide, sorbitol/mannitol</t>
+  </si>
+  <si>
+    <t>one carotenoid genes</t>
+  </si>
+  <si>
+    <t>fructose, glucose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nitrate/sulfonate/bicarbonate, sugar, xylose, arginine, amino acid, amino acid/amide (lots), arginine/ornithine, biotin, branched amino, carbohydrate, dipeptide, extacellular solute, glucose/mannose, heme, iron, LPS export, lipoprotein release, maltose, microcin C, molybdate, molybdenum, monosaccharide, nitrate/nitrite, phopholipid/cholesterol, phosphonate, putrescine, raffinose/stachyose/melibiose, ribose, sorbitol, sulfate, tungstate, urea, type II secretion </t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, sulfate oxidation (SOX), thiosulfate, alkane_sulfonate, methanesulfonate</t>
+  </si>
+  <si>
+    <t>nitrate_red_ass, , nitrogen fixation, nitroalkane, ammonia_assimilation</t>
+  </si>
+  <si>
+    <t>carbon fixation (RuBisCo), formate, MurNAc, fructose, glucose, sorbose, galactose, sucrose, glycolate, cellobiose, glucoside, starch/glycogen, trehalose, maltose, xylose</t>
   </si>
 </sst>
 </file>
@@ -3176,8 +3275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J114" workbookViewId="0">
-      <selection activeCell="M131" sqref="M131"/>
+    <sheetView tabSelected="1" topLeftCell="F132" workbookViewId="0">
+      <selection activeCell="K140" sqref="K140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9498,11 +9597,29 @@
       <c r="I132" s="1" t="s">
         <v>442</v>
       </c>
+      <c r="J132" t="s">
+        <v>919</v>
+      </c>
       <c r="M132" t="s">
         <v>488</v>
       </c>
+      <c r="N132" t="s">
+        <v>917</v>
+      </c>
       <c r="O132" t="s">
         <v>510</v>
+      </c>
+      <c r="P132" t="s">
+        <v>918</v>
+      </c>
+      <c r="Q132" t="s">
+        <v>916</v>
+      </c>
+      <c r="S132" t="s">
+        <v>839</v>
+      </c>
+      <c r="T132" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="133" spans="1:20" x14ac:dyDescent="0.25">
@@ -9533,8 +9650,26 @@
       <c r="I133" s="1" t="s">
         <v>443</v>
       </c>
+      <c r="J133" t="s">
+        <v>924</v>
+      </c>
+      <c r="L133" t="s">
+        <v>922</v>
+      </c>
       <c r="M133" t="s">
         <v>482</v>
+      </c>
+      <c r="N133" t="s">
+        <v>921</v>
+      </c>
+      <c r="P133" t="s">
+        <v>923</v>
+      </c>
+      <c r="Q133" t="s">
+        <v>920</v>
+      </c>
+      <c r="T133" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="134" spans="1:20" x14ac:dyDescent="0.25">
@@ -9565,11 +9700,26 @@
       <c r="I134" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="J134" t="s">
+        <v>926</v>
+      </c>
       <c r="M134" t="s">
         <v>469</v>
       </c>
+      <c r="N134" t="s">
+        <v>461</v>
+      </c>
       <c r="O134" t="s">
         <v>502</v>
+      </c>
+      <c r="P134" t="s">
+        <v>502</v>
+      </c>
+      <c r="Q134" t="s">
+        <v>925</v>
+      </c>
+      <c r="T134" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="135" spans="1:20" x14ac:dyDescent="0.25">
@@ -9600,11 +9750,32 @@
       <c r="I135" s="1" t="s">
         <v>454</v>
       </c>
+      <c r="J135" t="s">
+        <v>928</v>
+      </c>
+      <c r="K135" t="s">
+        <v>931</v>
+      </c>
       <c r="M135" t="s">
         <v>488</v>
       </c>
+      <c r="N135" t="s">
+        <v>929</v>
+      </c>
       <c r="O135" t="s">
         <v>510</v>
+      </c>
+      <c r="P135" t="s">
+        <v>930</v>
+      </c>
+      <c r="Q135" t="s">
+        <v>927</v>
+      </c>
+      <c r="S135" t="s">
+        <v>604</v>
+      </c>
+      <c r="T135" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="136" spans="1:20" x14ac:dyDescent="0.25">
@@ -9635,6 +9806,15 @@
       <c r="I136" s="1" t="s">
         <v>356</v>
       </c>
+      <c r="K136" t="s">
+        <v>933</v>
+      </c>
+      <c r="N136" t="s">
+        <v>791</v>
+      </c>
+      <c r="S136" t="s">
+        <v>932</v>
+      </c>
     </row>
     <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
@@ -9664,8 +9844,26 @@
       <c r="I137" s="1" t="s">
         <v>394</v>
       </c>
+      <c r="K137" t="s">
+        <v>935</v>
+      </c>
+      <c r="L137" t="s">
+        <v>937</v>
+      </c>
+      <c r="N137" t="s">
+        <v>936</v>
+      </c>
       <c r="O137" t="s">
         <v>502</v>
+      </c>
+      <c r="P137" t="s">
+        <v>653</v>
+      </c>
+      <c r="Q137" t="s">
+        <v>934</v>
+      </c>
+      <c r="T137" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="138" spans="1:20" x14ac:dyDescent="0.25">
@@ -9696,11 +9894,29 @@
       <c r="I138" s="1" t="s">
         <v>455</v>
       </c>
+      <c r="J138" t="s">
+        <v>941</v>
+      </c>
       <c r="M138" t="s">
         <v>489</v>
       </c>
+      <c r="N138" t="s">
+        <v>939</v>
+      </c>
       <c r="O138" t="s">
         <v>513</v>
+      </c>
+      <c r="P138" t="s">
+        <v>940</v>
+      </c>
+      <c r="Q138" t="s">
+        <v>938</v>
+      </c>
+      <c r="S138" t="s">
+        <v>826</v>
+      </c>
+      <c r="T138" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="139" spans="1:20" x14ac:dyDescent="0.25">
@@ -9731,8 +9947,26 @@
       <c r="I139" s="1" t="s">
         <v>397</v>
       </c>
+      <c r="J139" t="s">
+        <v>943</v>
+      </c>
+      <c r="K139" t="s">
+        <v>944</v>
+      </c>
       <c r="M139" t="s">
         <v>471</v>
+      </c>
+      <c r="N139" t="s">
+        <v>461</v>
+      </c>
+      <c r="P139" t="s">
+        <v>502</v>
+      </c>
+      <c r="Q139" t="s">
+        <v>942</v>
+      </c>
+      <c r="T139" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="140" spans="1:20" x14ac:dyDescent="0.25">
@@ -9763,11 +9997,29 @@
       <c r="I140" s="1" t="s">
         <v>398</v>
       </c>
+      <c r="J140" t="s">
+        <v>948</v>
+      </c>
       <c r="K140" t="s">
         <v>399</v>
       </c>
+      <c r="N140" t="s">
+        <v>947</v>
+      </c>
       <c r="O140" t="s">
         <v>502</v>
+      </c>
+      <c r="P140" t="s">
+        <v>946</v>
+      </c>
+      <c r="Q140" t="s">
+        <v>945</v>
+      </c>
+      <c r="S140" t="s">
+        <v>839</v>
+      </c>
+      <c r="T140" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="141" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added the stuff from my laptop today
</commit_message>
<xml_diff>
--- a/Data_files/combined_genome_data.xlsx
+++ b/Data_files/combined_genome_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2108" uniqueCount="949">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2181" uniqueCount="995">
   <si>
     <t>ME</t>
   </si>
@@ -2871,6 +2871,144 @@
   </si>
   <si>
     <t>carbon fixation (RuBisCo), formate, MurNAc, fructose, glucose, sorbose, galactose, sucrose, glycolate, cellobiose, glucoside, starch/glycogen, trehalose, maltose, xylose</t>
+  </si>
+  <si>
+    <t>three carotenoid biosynthesis genes, chitobiose, D-glucoseaminide, fructose, glucose, mannose, fructan, rhamnulose, rhamnose, galactose, raffinose, stachyose, manninotriose, melibiose, xylose, sucrose, glucoside, cellulose, cellobiose, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, one nitric oxide reductase</t>
+  </si>
+  <si>
+    <t>partial sulfate_red_ass, thiosulfate</t>
+  </si>
+  <si>
+    <t>xylose, iron, LPS export, lipoprotein release, phosphate, phospholipid/cholesterol, zinc</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose, rhamnose, rhamnulose, lactose, galactan, raffinose, stachyose, manninotriose, melibiose, glucoside, cellobiose, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>tetrathionate, one sulfite reductase, extracellular sulfate transport</t>
+  </si>
+  <si>
+    <t>xylose, iron, iron(III), LPS export, lipoprotein release, molybdate, oligopeptide, phosphate, phospholipid/cholesterol, sulfate, xylose</t>
+  </si>
+  <si>
+    <t>methanol, formate, chitobiose, fructose, glucose</t>
+  </si>
+  <si>
+    <t>partial sulfur oxidation (SOX)</t>
+  </si>
+  <si>
+    <t>LPS export, lipoprotein release, phosphate, phospholipid, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>chitobiose, MurNAc, glucose, glycolate, 1,3-B-glucan, glucoside, cellobiose, starch/glycogen, maltose, trehalose</t>
+  </si>
+  <si>
+    <t>nitrogen fixation, ammonia_assimilation, hydroxylamine, one nitrite reductase</t>
+  </si>
+  <si>
+    <t>sulfate_red_dis, thiosulfate, trithioniate</t>
+  </si>
+  <si>
+    <t>amino acid/amide, branched amino, cobalt/nickel, iron, LPS transport, microcin C, molybdate, phosphate, phospholipid, phospholipid/cholesterol, phosphonate, hydroxymethylpyrmidine, tungstate, zinc, type VI secretion</t>
+  </si>
+  <si>
+    <t>carotenoid biosynthesis, carbon fixation via Rubisco and reductive TCA, chitobiose, MurNAc, glucose, galacturonate, starch/glycogen, dextrin</t>
+  </si>
+  <si>
+    <t>nitrogen fixation, ammonia_assimilation, hydroxylamine</t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, trithionate, one sulfite reductase from sulfate_dis_ass</t>
+  </si>
+  <si>
+    <t>amino acid/amide, capsular polysaccharide, cobalt/nickel, iron, LPS export, lipoprotein release, molybdate, manganese/zinc/iron, macrolide, phosphate, phospholipid/cholesterol, sulfate</t>
+  </si>
+  <si>
+    <t>glucose, galactose, glycolate, glucoside, cellobiose, trehalose</t>
+  </si>
+  <si>
+    <t>taurine, sulfate_red_ass</t>
+  </si>
+  <si>
+    <t>amino acid/amide, branched amino, carbohydrate, heme, iron, LPS transport, phosphate, sn-glycerol 3-phosphate, spermidine/putrescine</t>
+  </si>
+  <si>
+    <t>partial Wood-Ljungdahl, glucose, fructan, glucoside, cellobiose</t>
+  </si>
+  <si>
+    <t>xylose, branched amino, iron (III), molybdate, monosaccharide, multiple sugar</t>
+  </si>
+  <si>
+    <t>Some oxidative phosphorylation</t>
+  </si>
+  <si>
+    <t>carbon fixation (RuBisCo), methanol, formate, acetate, MurNac, chitobiose, glycolate</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, nitrilase, nitronate monooxygenase</t>
+  </si>
+  <si>
+    <t>thiosulfate, partial sulfur oxidation (SOX)</t>
+  </si>
+  <si>
+    <t>branched amino, heme, LPS export, lipoprotein release, phosphate, phospholipid/cholesterol, type IV secretion</t>
+  </si>
+  <si>
+    <t>two flagellum proteins</t>
+  </si>
+  <si>
+    <t>MurNAC, chitobiose, glycolate</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, nitrilase</t>
+  </si>
+  <si>
+    <t>amino acid/amide, branched amino, heme, LPS export, lipoprotein release, microcin C, molybdate, paraquat-inducible, phosphate, phospholipid, phospholipid/cholesterol, tungstate</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose, galactose, rhamnulose, raffinose, stachyose, manninotriose, melibiose, glycolate, galacturonate, cellobiose, starch/glycogen, maltose, pectin, pectate</t>
+  </si>
+  <si>
+    <t>one sulfite reductase, thiosulfate</t>
+  </si>
+  <si>
+    <t>xylose, carbohydrate, iron, iron(III), LPS export, lipoprotein release, molybdate, oligopeptide, phosphate, phospholipid/cholesterol, sulfate, xylose</t>
+  </si>
+  <si>
+    <t>two carotenoid genes, glucose, glucoside, cellobiose, maltose</t>
+  </si>
+  <si>
+    <t>branched amino, xylose, biotin, iron, iron (III), monosaccharide, multiple sugar, phosphate, ribose, teichoic acid, thiamine</t>
+  </si>
+  <si>
+    <t>methanol, formaldehyde, formate, MurNAC, chitobiose, glucose, galacturonate, 1,3-B-glucan, glucoside, cellobiose, starch/glycogen, trehalose, maltose</t>
+  </si>
+  <si>
+    <t>heme, LPS export, lipoprotein release, molybdate, molybdenum, phosphate, phospholipid/cholesterol, phosphonate, sulfate</t>
+  </si>
+  <si>
+    <t>methanol, formaldehyde, formate, MurNAc, chitobiose, glycolate, starch/glycogen</t>
+  </si>
+  <si>
+    <t>LPS export, oligopeptide, phosphate, phospholipid, phospholipid/cholesterol, putrescine</t>
+  </si>
+  <si>
+    <t>partial Wood-Ljungdahl</t>
+  </si>
+  <si>
+    <t>chitobiose, glycolate, xylose, glucoside, cellobiose, cellulose</t>
+  </si>
+  <si>
+    <t>sulfur oxidation (SOX)</t>
+  </si>
+  <si>
+    <t>carbohydrate, glycine betaine/proline, heme, lipoprotein release, molybdate, osmoprotectant, phosphate, phospholipid/cholesterol, phospholipid, putrescine, sodium, spermidine/putrescine</t>
+  </si>
+  <si>
+    <t>chemotaxis (purine?)</t>
   </si>
 </sst>
 </file>
@@ -3275,8 +3413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F132" workbookViewId="0">
-      <selection activeCell="K140" sqref="K140"/>
+    <sheetView tabSelected="1" topLeftCell="D159" workbookViewId="0">
+      <selection activeCell="A190" sqref="A190:XFD203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11166,7 +11304,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>2582580703</v>
       </c>
@@ -11198,7 +11336,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>2582580704</v>
       </c>
@@ -11225,7 +11363,7 @@
       </c>
       <c r="I178" s="1"/>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>2582580705</v>
       </c>
@@ -11257,7 +11395,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>2582580706</v>
       </c>
@@ -11284,7 +11422,7 @@
       </c>
       <c r="I180" s="1"/>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>2582580707</v>
       </c>
@@ -11319,7 +11457,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>2582580708</v>
       </c>
@@ -11348,7 +11486,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>2582580709</v>
       </c>
@@ -11375,7 +11513,7 @@
       </c>
       <c r="I183" s="1"/>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>2582580711</v>
       </c>
@@ -11405,7 +11543,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>2582580712</v>
       </c>
@@ -11440,7 +11578,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>2582580714</v>
       </c>
@@ -11467,7 +11605,7 @@
       </c>
       <c r="I186" s="1"/>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>2593339176</v>
       </c>
@@ -11499,7 +11637,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>2593339177</v>
       </c>
@@ -11534,7 +11672,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>2593339178</v>
       </c>
@@ -11569,7 +11707,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>2593339179</v>
       </c>
@@ -11597,14 +11735,32 @@
       <c r="I190" s="1" t="s">
         <v>417</v>
       </c>
+      <c r="J190" t="s">
+        <v>949</v>
+      </c>
       <c r="M190" t="s">
         <v>474</v>
       </c>
+      <c r="N190" t="s">
+        <v>950</v>
+      </c>
       <c r="O190" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P190" t="s">
+        <v>951</v>
+      </c>
+      <c r="Q190" t="s">
+        <v>952</v>
+      </c>
+      <c r="R190" t="s">
+        <v>604</v>
+      </c>
+      <c r="T190" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="191" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>2593339181</v>
       </c>
@@ -11632,8 +11788,23 @@
       <c r="I191" s="1" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J191" t="s">
+        <v>953</v>
+      </c>
+      <c r="N191" t="s">
+        <v>461</v>
+      </c>
+      <c r="P191" t="s">
+        <v>954</v>
+      </c>
+      <c r="Q191" t="s">
+        <v>955</v>
+      </c>
+      <c r="T191" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="192" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>2593339182</v>
       </c>
@@ -11659,8 +11830,23 @@
         <v>2582580649</v>
       </c>
       <c r="I192" s="1"/>
-    </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J192" t="s">
+        <v>956</v>
+      </c>
+      <c r="N192" t="s">
+        <v>921</v>
+      </c>
+      <c r="P192" t="s">
+        <v>957</v>
+      </c>
+      <c r="Q192" t="s">
+        <v>958</v>
+      </c>
+      <c r="T192" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="193" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>2593339183</v>
       </c>
@@ -11688,11 +11874,29 @@
       <c r="I193" s="1" t="s">
         <v>388</v>
       </c>
+      <c r="J193" t="s">
+        <v>959</v>
+      </c>
       <c r="M193" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N193" t="s">
+        <v>960</v>
+      </c>
+      <c r="P193" t="s">
+        <v>961</v>
+      </c>
+      <c r="Q193" t="s">
+        <v>962</v>
+      </c>
+      <c r="R193" t="s">
+        <v>839</v>
+      </c>
+      <c r="T193" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>2593339184</v>
       </c>
@@ -11720,14 +11924,32 @@
       <c r="I194" s="1" t="s">
         <v>453</v>
       </c>
+      <c r="J194" t="s">
+        <v>963</v>
+      </c>
       <c r="M194" t="s">
         <v>485</v>
       </c>
+      <c r="N194" t="s">
+        <v>964</v>
+      </c>
       <c r="O194" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P194" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q194" t="s">
+        <v>966</v>
+      </c>
+      <c r="R194" t="s">
+        <v>604</v>
+      </c>
+      <c r="T194" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="195" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>2593339185</v>
       </c>
@@ -11755,8 +11977,23 @@
       <c r="I195" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J195" t="s">
+        <v>967</v>
+      </c>
+      <c r="N195" t="s">
+        <v>461</v>
+      </c>
+      <c r="P195" t="s">
+        <v>968</v>
+      </c>
+      <c r="Q195" t="s">
+        <v>969</v>
+      </c>
+      <c r="T195" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="196" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>2593339186</v>
       </c>
@@ -11782,8 +12019,20 @@
         <v>2593339190</v>
       </c>
       <c r="I196" s="1"/>
-    </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J196" t="s">
+        <v>970</v>
+      </c>
+      <c r="N196" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q196" t="s">
+        <v>971</v>
+      </c>
+      <c r="T196" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="197" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>2593339187</v>
       </c>
@@ -11811,11 +12060,29 @@
       <c r="I197" s="1" t="s">
         <v>451</v>
       </c>
+      <c r="J197" t="s">
+        <v>973</v>
+      </c>
+      <c r="N197" t="s">
+        <v>974</v>
+      </c>
       <c r="O197" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P197" t="s">
+        <v>975</v>
+      </c>
+      <c r="Q197" t="s">
+        <v>976</v>
+      </c>
+      <c r="R197" t="s">
+        <v>977</v>
+      </c>
+      <c r="T197" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="198" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>2593339188</v>
       </c>
@@ -11841,11 +12108,23 @@
         <v>342</v>
       </c>
       <c r="I198" s="1"/>
+      <c r="J198" t="s">
+        <v>978</v>
+      </c>
+      <c r="N198" t="s">
+        <v>979</v>
+      </c>
       <c r="O198" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q198" t="s">
+        <v>980</v>
+      </c>
+      <c r="T198" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="199" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>2593339189</v>
       </c>
@@ -11873,8 +12152,23 @@
       <c r="I199" s="1" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J199" t="s">
+        <v>981</v>
+      </c>
+      <c r="N199" t="s">
+        <v>791</v>
+      </c>
+      <c r="P199" t="s">
+        <v>982</v>
+      </c>
+      <c r="Q199" t="s">
+        <v>983</v>
+      </c>
+      <c r="T199" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="200" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>2593339190</v>
       </c>
@@ -11900,8 +12194,20 @@
         <v>2593339186</v>
       </c>
       <c r="I200" s="1"/>
-    </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J200" t="s">
+        <v>984</v>
+      </c>
+      <c r="N200" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q200" t="s">
+        <v>985</v>
+      </c>
+      <c r="T200" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="201" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>2593339191</v>
       </c>
@@ -11929,11 +12235,29 @@
       <c r="I201" s="1" t="s">
         <v>452</v>
       </c>
+      <c r="J201" t="s">
+        <v>986</v>
+      </c>
+      <c r="N201" t="s">
+        <v>921</v>
+      </c>
       <c r="O201" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P201" t="s">
+        <v>653</v>
+      </c>
+      <c r="Q201" t="s">
+        <v>987</v>
+      </c>
+      <c r="R201" t="s">
+        <v>839</v>
+      </c>
+      <c r="T201" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="202" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>2593339192</v>
       </c>
@@ -11961,11 +12285,23 @@
       <c r="I202" s="1" t="s">
         <v>390</v>
       </c>
+      <c r="J202" t="s">
+        <v>988</v>
+      </c>
       <c r="M202" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N202" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q202" t="s">
+        <v>989</v>
+      </c>
+      <c r="T202" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="203" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>2593339193</v>
       </c>
@@ -11993,14 +12329,35 @@
       <c r="I203" s="1" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J203" t="s">
+        <v>990</v>
+      </c>
+      <c r="L203" t="s">
+        <v>991</v>
+      </c>
+      <c r="N203" t="s">
+        <v>461</v>
+      </c>
+      <c r="P203" t="s">
+        <v>992</v>
+      </c>
+      <c r="Q203" t="s">
+        <v>993</v>
+      </c>
+      <c r="R203" t="s">
+        <v>994</v>
+      </c>
+      <c r="T203" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="204" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I204" s="1"/>
     </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I205" s="1"/>
     </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I206" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3/4 done with genomes!
</commit_message>
<xml_diff>
--- a/Data_files/combined_genome_data.xlsx
+++ b/Data_files/combined_genome_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\MAGstravaganza\Data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amlin\Desktop\MAGstravaganza\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2235" uniqueCount="1025">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2273" uniqueCount="1044">
   <si>
     <t>ME</t>
   </si>
@@ -3099,12 +3099,69 @@
   </si>
   <si>
     <t>formate, chitobiose, MurNAc, glucose, sucrose, tartrate, glycolate, maltose, dextrin, starch/glycogen</t>
+  </si>
+  <si>
+    <t>iron, LPS export, lipoprotein release, phosphate, phospholipid/cholesterol, zinc</t>
+  </si>
+  <si>
+    <t>chitobiose, glucosaminide, fructose, arabinose, glucose, galactose, mannose, fructan, rhamnose, rhamnulose, fucose, fuculose, raffinose, stachyose, manninotriose, melibose, sucrose, glucoside, cellobiose, pectin, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>amino acid/amide, fructose, heme, LPS export, lipoprotein release, molybdate, phosphate, phospholipid, phosphonate, ribose, sulfate</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, nitrilase, partial denitrification</t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, sulfate_red_dis, sulfur oxidation (SOX), trithionate</t>
+  </si>
+  <si>
+    <t>formate, MurNAc, chitobiose, fructose, glucose, cellulose degradation and biosynthesis, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>amino acid/amide, biotin, carbohydrate, glycine betaine/proline, iron, iron(III), molybdate, monosaccharide, phosphate, raffinose/stachyose/melibiose, rhamnose, teichoic acid, thiol reductant</t>
+  </si>
+  <si>
+    <t>two carotenoid genes, formate, fructose, glucose, galactose, rhamnose, rhamnulose, raffinose, stachyose, manninotriose, melibiose, sucrose, cellobiose, glucoside, maltose</t>
+  </si>
+  <si>
+    <t>nitrogen_fixation, ammonia_assimilation, nitrite reductase, nitrate reductase</t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, alkane_sulfonate, methanesulfonate, thiosulfate</t>
+  </si>
+  <si>
+    <t>methane, methanol, formate, chitobiose, fructose, glucose, glycolate, glucoside, 1,3-B-glucan, cellobiose, galacturonate, maltose, starch/glycogen, trehalose</t>
+  </si>
+  <si>
+    <t>LPS tranport</t>
+  </si>
+  <si>
+    <t>bacitracin, biotin, carbohydrate, cobalt/nickel, heme, iron, lipoprotein release, molybdate, oligopeptide, peptide/nickel, phosphate, polar amino acid, taurine</t>
+  </si>
+  <si>
+    <t>nitrogen_fixation, ammonia_assimilation, nitronate</t>
+  </si>
+  <si>
+    <t>Wood-Ljungdahl (complete!), trimethylamine, formate, glyoxylate, glucose, sucrose, stachyose, raffinose, manninotriose, melibiose, cellulose, trehalose</t>
+  </si>
+  <si>
+    <t>methionine, amino acid/amide, carbohydrate, cobalt/nickel, iron, LpS export, lipoprotein release, oligopeptide, phosphate, phospholipid/cholesterol, spermidine/putrescine, sulfate, sulfonate, zinc</t>
+  </si>
+  <si>
+    <t>nitrogen_fixation, ammonia_assimilation, nitrite reductase</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose, galactose, rhamnulose, rhamnose, fucose, fuculose, lactose, stachyose, raffinose, sucrose, manninotriose, meliobiose, glycolate, glucoside, cellulose, cellobiose, starch/glycogen, dextrin</t>
+  </si>
+  <si>
+    <t>biotin, heme, LPS export, lipoprotein release, phospholipid, phospholipid/cholesterol, spermidine/putrescine, zinc, type IV secretion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3503,8 +3560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="K150" sqref="K150"/>
+    <sheetView tabSelected="1" topLeftCell="H135" workbookViewId="0">
+      <selection activeCell="K158" sqref="K158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10767,8 +10824,26 @@
       <c r="I151" s="1" t="s">
         <v>405</v>
       </c>
+      <c r="J151" t="s">
+        <v>1026</v>
+      </c>
+      <c r="N151" t="s">
+        <v>461</v>
+      </c>
       <c r="O151" t="s">
         <v>508</v>
+      </c>
+      <c r="P151" t="s">
+        <v>502</v>
+      </c>
+      <c r="Q151" t="s">
+        <v>1025</v>
+      </c>
+      <c r="S151" t="s">
+        <v>604</v>
+      </c>
+      <c r="T151" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="152" spans="1:20" x14ac:dyDescent="0.25">
@@ -10799,8 +10874,26 @@
       <c r="I152" s="1" t="s">
         <v>406</v>
       </c>
+      <c r="J152" t="s">
+        <v>1030</v>
+      </c>
+      <c r="N152" t="s">
+        <v>1028</v>
+      </c>
       <c r="O152" t="s">
         <v>517</v>
+      </c>
+      <c r="P152" t="s">
+        <v>1029</v>
+      </c>
+      <c r="Q152" t="s">
+        <v>1027</v>
+      </c>
+      <c r="S152" t="s">
+        <v>813</v>
+      </c>
+      <c r="T152" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="153" spans="1:20" x14ac:dyDescent="0.25">
@@ -10831,8 +10924,20 @@
       <c r="I153" s="1" t="s">
         <v>356</v>
       </c>
+      <c r="J153" t="s">
+        <v>1032</v>
+      </c>
+      <c r="N153" t="s">
+        <v>461</v>
+      </c>
       <c r="O153" t="s">
         <v>502</v>
+      </c>
+      <c r="Q153" t="s">
+        <v>1031</v>
+      </c>
+      <c r="T153" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="154" spans="1:20" x14ac:dyDescent="0.25">
@@ -10863,11 +10968,26 @@
       <c r="I154" s="1" t="s">
         <v>407</v>
       </c>
+      <c r="J154" t="s">
+        <v>1035</v>
+      </c>
       <c r="M154" t="s">
         <v>486</v>
       </c>
+      <c r="N154" t="s">
+        <v>1033</v>
+      </c>
       <c r="O154" t="s">
         <v>502</v>
+      </c>
+      <c r="P154" t="s">
+        <v>1034</v>
+      </c>
+      <c r="Q154" t="s">
+        <v>836</v>
+      </c>
+      <c r="T154" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="155" spans="1:20" x14ac:dyDescent="0.25">
@@ -10896,6 +11016,18 @@
         <v>342</v>
       </c>
       <c r="I155" s="1"/>
+      <c r="N155" t="s">
+        <v>461</v>
+      </c>
+      <c r="P155" t="s">
+        <v>502</v>
+      </c>
+      <c r="Q155" t="s">
+        <v>1036</v>
+      </c>
+      <c r="T155" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="156" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
@@ -10925,11 +11057,23 @@
       <c r="I156" s="1" t="s">
         <v>408</v>
       </c>
+      <c r="J156" t="s">
+        <v>1039</v>
+      </c>
       <c r="M156" t="s">
         <v>486</v>
       </c>
+      <c r="N156" t="s">
+        <v>1038</v>
+      </c>
       <c r="O156" t="s">
         <v>508</v>
+      </c>
+      <c r="Q156" t="s">
+        <v>1037</v>
+      </c>
+      <c r="T156" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="157" spans="1:20" x14ac:dyDescent="0.25">
@@ -10960,8 +11104,23 @@
       <c r="I157" s="1" t="s">
         <v>409</v>
       </c>
+      <c r="J157" t="s">
+        <v>1042</v>
+      </c>
       <c r="M157" t="s">
         <v>488</v>
+      </c>
+      <c r="N157" t="s">
+        <v>1041</v>
+      </c>
+      <c r="P157" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q157" t="s">
+        <v>1040</v>
+      </c>
+      <c r="T157" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="158" spans="1:20" x14ac:dyDescent="0.25">
@@ -10990,8 +11149,20 @@
         <v>2582580644</v>
       </c>
       <c r="I158" s="1"/>
+      <c r="J158" t="s">
+        <v>797</v>
+      </c>
       <c r="M158" t="s">
         <v>461</v>
+      </c>
+      <c r="N158" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q158" t="s">
+        <v>1043</v>
+      </c>
+      <c r="T158" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="159" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Only 14 genomes left!
</commit_message>
<xml_diff>
--- a/Data_files/combined_genome_data.xlsx
+++ b/Data_files/combined_genome_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amlin\Desktop\MAGstravaganza\Data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\MAGstravaganza\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2273" uniqueCount="1044">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2362" uniqueCount="1092">
   <si>
     <t>ME</t>
   </si>
@@ -3156,12 +3156,156 @@
   </si>
   <si>
     <t>biotin, heme, LPS export, lipoprotein release, phospholipid, phospholipid/cholesterol, spermidine/putrescine, zinc, type IV secretion</t>
+  </si>
+  <si>
+    <t>branched amino, amino acid/amide, cobalt/nickel, L-amino, iron, LPS export, lipoprotein release, microcin C, multiple sugar, molybdate, phosphate, phospholipid/cholesterol, phosphonate, tungstate</t>
+  </si>
+  <si>
+    <t>nitrate reduction, nitrogen fixation, ammonia_assimilation, hydroxylamine reductase</t>
+  </si>
+  <si>
+    <t>sulfate_red_dis, trithionate</t>
+  </si>
+  <si>
+    <t>Cu-processing, heme, LPS export, lipoprotein release, molybdate, phosphate, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>partial denitrification, ammonia_assimilation</t>
+  </si>
+  <si>
+    <t>three carotenoid genes, chitobiose, fructose, glucose, galactose, sucrose, glucoside, cellulose, cellobiose, starch/glycogen, trehalsoe, maltose, dextrin, isomaltose</t>
+  </si>
+  <si>
+    <t>peptidase, arginine, biotin, LPS export, lipoprotein release, macrolide, phospholipid/cholesterol, putative hydroxymethylpyrimidine, spermidine/putrescine, type IV secretion</t>
+  </si>
+  <si>
+    <t>chitobiose, fructose, starch/glycogen, trehalose</t>
+  </si>
+  <si>
+    <t>amino acid/amide, branched amino, cobalt/nickel, iron, LPS export, lipoprotein release, maltose/maltodextrin, molybdate, multiple sugar, phosphate, phospholipid/cholesterol, sodium, tungstate, type VI secretion</t>
+  </si>
+  <si>
+    <t>nitrate_red_diss, partial denitrification, ammonia_assimilation</t>
+  </si>
+  <si>
+    <t>sufate_red_ass, thiosulfate, tetrathionate</t>
+  </si>
+  <si>
+    <t>chitin, chitobiose, MurNAc, fructose, glucose, sucrose, stachyose, raffinose, glycolate, glycerate, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>branched amino, MacB-like domain, NAG, amino acid/amide, carbohydrate, cobalt/nickel, extracellular, iron, iron (III), lactose/arabinose, LPS export, lipoprotein release, molybdate, monosaccharide, multiple sugar, oligopeptide, phosphate, phospholipid/cholesterol, raffinose/stachyose/melibiose, sodium, xylose, type IV secretion</t>
+  </si>
+  <si>
+    <t>nitrate reduction, ammonia_assimilation</t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, trithionate</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose, galactose, sorbose, sorbitol, rhamnose, rhamnulose, raffinose/stachyose/manninotriose, melibiose, tartrate, glycolate, trehalose, galacturonate,  cellulose, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>branched amino, polysaccharide/polyol phosphate export, cobalt, permease, zinc, amino acid/amide, cobalamin, cobalt/nickel, LPS export, lipoprotein release, macrolide, molybdate, molybdenum, phosphate, phospholipid/cholesterol, sulfate, tungstate, zinc, type II secretion, type VI secretion</t>
+  </si>
+  <si>
+    <t>partial Wood-Ljungdahl, acetate, formaldehyde, formate</t>
+  </si>
+  <si>
+    <t>nitrate_red_dis, partial denitrification, nitrogen fixation, ammonia_assimilation</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose, tartrate, glycolate, glycerate, cellulose, galacturonate, starch/glycogen, dextrin, trehalose, maltose</t>
+  </si>
+  <si>
+    <t>Cu-processing, permease, LPS export, lipoprotein release, phosphate, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>two carotenoid genes, galactose, fructan, sucrose, cellobiose, cellulose synthesis, maltose</t>
+  </si>
+  <si>
+    <t>cobalt, iron, LPS export, lipoprotein, oligopeptide/dipeptide, phospholipid/cholesterol, sulfate</t>
+  </si>
+  <si>
+    <t>nitrite reducatse, nitroalkane, ammonia_assimilation, hydroxylamine reductase</t>
+  </si>
+  <si>
+    <t>chitobiose, fructose, galactose, fructan, sorbitol, rhamnulose, raffinose, stachyose, manninotriose, meliobiose, sucrose, galactan, glucoside, cellulose, cellobiose, starch/glycogen, pectin, maltose</t>
+  </si>
+  <si>
+    <t>permease, LPS export, lipoprotein release, molybdate, phosphate, phospholipid, ribose, sulfonate, ribose</t>
+  </si>
+  <si>
+    <t>alkanesulfonate, methanesulfonate, sulfite reductaase</t>
+  </si>
+  <si>
+    <t>chitobiose, fructose, glucose, fructan, rhamnose, rhamnulose, galactose, galactan, lactose, raffinose, stachyose, manninotriose, melibiose,,pectin, cellobiose, glucoside, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>LPS transport</t>
+  </si>
+  <si>
+    <t>MacB-like domain, permease, heme, LPS export, lipoprotein, molybdate, phosphate, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>partial Wood-Ljungdahl, acetate, formate</t>
+  </si>
+  <si>
+    <t>nitrite reductase, ammonia_assimilation</t>
+  </si>
+  <si>
+    <t>a few chemotaxis protein</t>
+  </si>
+  <si>
+    <t>NitT/TauT, permease, heme, iron, LPS export, lipoprotein release, macrolide, molybdate, peptide/nickel, phosphate, phospholipid/cholesterol, phosphonate, tungstate/molybdate, zinc</t>
+  </si>
+  <si>
+    <t>one carotenoid gene, formate, partial Wood-Ljungdahl, acetate</t>
+  </si>
+  <si>
+    <t>nitrite reductase, nitric oxide reductase, ammonia_assimilation</t>
+  </si>
+  <si>
+    <t>chitin, chitobiose, fructose, glucose, galactose, fructan, fucose , fuculose, rhamnose, rhamnulose, lactose, galactan, raffinose, stachyose, manninotriose, melibiose, sucrose, pectin, glucoside, cellobiose, maltose, trehalose</t>
+  </si>
+  <si>
+    <t>NitT/TauT, biotin, branched amino, carbohydrate, heme, LPS export, lipoprotein release, molybdate, phosphate, phospholipid/cholesterol, zinc</t>
+  </si>
+  <si>
+    <t>chitin, chitobiose, glucosaminide, fructose, galactan, lactose, sucrose, glycerate, cellobiose, glucoside, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>chitobiose, MurNAc, glucoside, cellobiose</t>
+  </si>
+  <si>
+    <t>a few chemotaxis proteins, flagellum</t>
+  </si>
+  <si>
+    <t>chitobiose, MurNAc</t>
+  </si>
+  <si>
+    <t>HCOMODA decarboxylase, amino acid/amide, glutamate, branched amino, L-amino, glycine betaine/choline, heme, iron, iron(III), LPS export, lipoprotein release, molybdate, multiple sugar, nitrate/nitrite, phosphate, phospholipid/cholesterol, polar amino, sulfonate, tungstate, urea</t>
+  </si>
+  <si>
+    <t>Some carotenoid genes, partial Wood-Ljungdahl, acetate, formate</t>
+  </si>
+  <si>
+    <t>nitrate reductase, nitrite reductase, ammonia_assimilation, formamide, nitroalkane, nitrile</t>
+  </si>
+  <si>
+    <t>sulfate oxidation, taurine, alkanesulfonate, methanesulfonate, thiosulfate</t>
+  </si>
+  <si>
+    <t>a few chemotaxis and flagellum proteins</t>
+  </si>
+  <si>
+    <t>chitobiose, fructose, galactose, galactonate, tartrate, glycerate, glycolate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3560,8 +3704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H135" workbookViewId="0">
-      <selection activeCell="K158" sqref="K158"/>
+    <sheetView tabSelected="1" topLeftCell="J159" workbookViewId="0">
+      <selection activeCell="M174" sqref="M174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11191,8 +11335,26 @@
         <v>342</v>
       </c>
       <c r="I159" s="1"/>
+      <c r="J159" t="s">
+        <v>959</v>
+      </c>
+      <c r="N159" t="s">
+        <v>1045</v>
+      </c>
       <c r="O159" t="s">
         <v>502</v>
+      </c>
+      <c r="P159" t="s">
+        <v>1046</v>
+      </c>
+      <c r="Q159" t="s">
+        <v>1044</v>
+      </c>
+      <c r="S159" t="s">
+        <v>826</v>
+      </c>
+      <c r="T159" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="160" spans="1:20" x14ac:dyDescent="0.25">
@@ -11223,8 +11385,23 @@
       <c r="I160" s="1" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J160" t="s">
+        <v>1049</v>
+      </c>
+      <c r="N160" t="s">
+        <v>1048</v>
+      </c>
+      <c r="Q160" t="s">
+        <v>1047</v>
+      </c>
+      <c r="S160" t="s">
+        <v>604</v>
+      </c>
+      <c r="T160" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="161" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>2582580686</v>
       </c>
@@ -11252,8 +11429,20 @@
       <c r="I161" s="1" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J161" t="s">
+        <v>1051</v>
+      </c>
+      <c r="N161" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q161" t="s">
+        <v>1050</v>
+      </c>
+      <c r="T161" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="162" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>2582580687</v>
       </c>
@@ -11281,14 +11470,32 @@
       <c r="I162" s="1" t="s">
         <v>411</v>
       </c>
+      <c r="J162" t="s">
+        <v>1055</v>
+      </c>
       <c r="M162" t="s">
         <v>482</v>
       </c>
+      <c r="N162" t="s">
+        <v>1053</v>
+      </c>
       <c r="O162" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P162" t="s">
+        <v>1054</v>
+      </c>
+      <c r="Q162" t="s">
+        <v>1052</v>
+      </c>
+      <c r="S162" t="s">
+        <v>839</v>
+      </c>
+      <c r="T162" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="163" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>2582580688</v>
       </c>
@@ -11316,11 +11523,26 @@
       <c r="I163" s="1" t="s">
         <v>413</v>
       </c>
+      <c r="J163" t="s">
+        <v>1059</v>
+      </c>
+      <c r="N163" t="s">
+        <v>1057</v>
+      </c>
       <c r="O163" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P163" t="s">
+        <v>1058</v>
+      </c>
+      <c r="Q163" t="s">
+        <v>1056</v>
+      </c>
+      <c r="T163" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="164" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>2582580689</v>
       </c>
@@ -11348,14 +11570,35 @@
       <c r="I164" s="1" t="s">
         <v>346</v>
       </c>
+      <c r="J164" t="s">
+        <v>1061</v>
+      </c>
+      <c r="L164" t="s">
+        <v>1063</v>
+      </c>
       <c r="M164" t="s">
         <v>492</v>
       </c>
+      <c r="N164" t="s">
+        <v>1062</v>
+      </c>
       <c r="O164" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P164" t="s">
+        <v>653</v>
+      </c>
+      <c r="Q164" t="s">
+        <v>1060</v>
+      </c>
+      <c r="S164" t="s">
+        <v>839</v>
+      </c>
+      <c r="T164" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="165" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>2582580690</v>
       </c>
@@ -11383,8 +11626,23 @@
       <c r="I165" s="1" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J165" t="s">
+        <v>1065</v>
+      </c>
+      <c r="N165" t="s">
+        <v>1048</v>
+      </c>
+      <c r="Q165" t="s">
+        <v>1064</v>
+      </c>
+      <c r="S165" t="s">
+        <v>604</v>
+      </c>
+      <c r="T165" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="166" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>2582580691</v>
       </c>
@@ -11412,14 +11670,32 @@
       <c r="I166" s="1" t="s">
         <v>414</v>
       </c>
+      <c r="J166" t="s">
+        <v>1068</v>
+      </c>
       <c r="M166" t="s">
         <v>493</v>
       </c>
+      <c r="N166" t="s">
+        <v>1067</v>
+      </c>
       <c r="O166" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P166" t="s">
+        <v>1009</v>
+      </c>
+      <c r="Q166" t="s">
+        <v>1066</v>
+      </c>
+      <c r="S166" t="s">
+        <v>994</v>
+      </c>
+      <c r="T166" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="167" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>2582580692</v>
       </c>
@@ -11447,11 +11723,29 @@
       <c r="I167" s="1" t="s">
         <v>499</v>
       </c>
+      <c r="J167" t="s">
+        <v>1071</v>
+      </c>
       <c r="M167" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N167" t="s">
+        <v>864</v>
+      </c>
+      <c r="P167" t="s">
+        <v>1070</v>
+      </c>
+      <c r="Q167" t="s">
+        <v>1069</v>
+      </c>
+      <c r="S167" t="s">
+        <v>604</v>
+      </c>
+      <c r="T167" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="168" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>2582580693</v>
       </c>
@@ -11477,8 +11771,14 @@
         <v>342</v>
       </c>
       <c r="I168" s="1"/>
-    </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q168" t="s">
+        <v>1072</v>
+      </c>
+      <c r="T168" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="169" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>2582580694</v>
       </c>
@@ -11504,8 +11804,29 @@
         <v>342</v>
       </c>
       <c r="I169" s="1"/>
-    </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J169" t="s">
+        <v>1074</v>
+      </c>
+      <c r="L169" t="s">
+        <v>827</v>
+      </c>
+      <c r="N169" t="s">
+        <v>1075</v>
+      </c>
+      <c r="P169" t="s">
+        <v>653</v>
+      </c>
+      <c r="Q169" t="s">
+        <v>1073</v>
+      </c>
+      <c r="S169" t="s">
+        <v>1076</v>
+      </c>
+      <c r="T169" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="170" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>2582580695</v>
       </c>
@@ -11533,14 +11854,35 @@
       <c r="I170" s="1" t="s">
         <v>447</v>
       </c>
+      <c r="J170" t="s">
+        <v>1078</v>
+      </c>
+      <c r="L170" t="s">
+        <v>1080</v>
+      </c>
       <c r="M170" t="s">
         <v>494</v>
       </c>
+      <c r="N170" t="s">
+        <v>1079</v>
+      </c>
       <c r="O170" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P170" t="s">
+        <v>502</v>
+      </c>
+      <c r="Q170" t="s">
+        <v>1077</v>
+      </c>
+      <c r="S170" t="s">
+        <v>839</v>
+      </c>
+      <c r="T170" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="171" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>2582580697</v>
       </c>
@@ -11568,14 +11910,35 @@
       <c r="I171" s="1" t="s">
         <v>415</v>
       </c>
+      <c r="J171" t="s">
+        <v>1074</v>
+      </c>
+      <c r="L171" t="s">
+        <v>1082</v>
+      </c>
       <c r="M171" t="s">
         <v>493</v>
       </c>
+      <c r="N171" t="s">
+        <v>1079</v>
+      </c>
       <c r="O171" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P171" t="s">
+        <v>634</v>
+      </c>
+      <c r="Q171" t="s">
+        <v>1081</v>
+      </c>
+      <c r="S171" t="s">
+        <v>604</v>
+      </c>
+      <c r="T171" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="172" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>2582580698</v>
       </c>
@@ -11601,8 +11964,20 @@
         <v>2582580629</v>
       </c>
       <c r="I172" s="1"/>
-    </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J172" t="s">
+        <v>1083</v>
+      </c>
+      <c r="N172" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q172" t="s">
+        <v>909</v>
+      </c>
+      <c r="T172" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="173" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>2582580699</v>
       </c>
@@ -11628,11 +12003,26 @@
         <v>2582580624</v>
       </c>
       <c r="I173" s="1"/>
+      <c r="J173" t="s">
+        <v>1085</v>
+      </c>
       <c r="M173" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N173" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q173" t="s">
+        <v>861</v>
+      </c>
+      <c r="S173" t="s">
+        <v>1084</v>
+      </c>
+      <c r="T173" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="174" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>2582580700</v>
       </c>
@@ -11658,14 +12048,35 @@
         <v>342</v>
       </c>
       <c r="I174" s="1"/>
+      <c r="J174" t="s">
+        <v>1087</v>
+      </c>
       <c r="K174" t="s">
         <v>399</v>
       </c>
+      <c r="L174" t="s">
+        <v>1091</v>
+      </c>
+      <c r="N174" t="s">
+        <v>1088</v>
+      </c>
       <c r="O174" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P174" t="s">
+        <v>1089</v>
+      </c>
+      <c r="Q174" t="s">
+        <v>1086</v>
+      </c>
+      <c r="S174" t="s">
+        <v>1090</v>
+      </c>
+      <c r="T174" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="175" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>2582580701</v>
       </c>
@@ -11692,7 +12103,7 @@
       </c>
       <c r="I175" s="1"/>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>2582580702</v>
       </c>
@@ -12176,7 +12587,7 @@
       <c r="Q190" t="s">
         <v>952</v>
       </c>
-      <c r="R190" t="s">
+      <c r="S190" t="s">
         <v>604</v>
       </c>
       <c r="T190" t="s">
@@ -12312,7 +12723,7 @@
       <c r="Q193" t="s">
         <v>962</v>
       </c>
-      <c r="R193" t="s">
+      <c r="S193" t="s">
         <v>839</v>
       </c>
       <c r="T193" t="s">
@@ -12365,7 +12776,7 @@
       <c r="Q194" t="s">
         <v>966</v>
       </c>
-      <c r="R194" t="s">
+      <c r="S194" t="s">
         <v>604</v>
       </c>
       <c r="T194" t="s">
@@ -12498,7 +12909,7 @@
       <c r="Q197" t="s">
         <v>976</v>
       </c>
-      <c r="R197" t="s">
+      <c r="S197" t="s">
         <v>977</v>
       </c>
       <c r="T197" t="s">
@@ -12673,7 +13084,7 @@
       <c r="Q201" t="s">
         <v>987</v>
       </c>
-      <c r="R201" t="s">
+      <c r="S201" t="s">
         <v>839</v>
       </c>
       <c r="T201" t="s">
@@ -12767,7 +13178,7 @@
       <c r="Q203" t="s">
         <v>993</v>
       </c>
-      <c r="R203" t="s">
+      <c r="S203" t="s">
         <v>994</v>
       </c>
       <c r="T203" t="s">

</xml_diff>

<commit_message>
Finished IMG analysis of all genomesgit add Data_files/combined_genome_data.xlsx !
</commit_message>
<xml_diff>
--- a/Data_files/combined_genome_data.xlsx
+++ b/Data_files/combined_genome_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2362" uniqueCount="1092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2444" uniqueCount="1134">
   <si>
     <t>ME</t>
   </si>
@@ -3300,6 +3300,132 @@
   </si>
   <si>
     <t>chitobiose, fructose, galactose, galactonate, tartrate, glycerate, glycolate</t>
+  </si>
+  <si>
+    <t>iron, LPS export, lipoprotein release, macrolidde, phosphate, phospholipid/cholesterol, zinc</t>
+  </si>
+  <si>
+    <t>three carotenoid genes, partial Wood-Ljungdahl, acetate</t>
+  </si>
+  <si>
+    <t>nitric oxide reductase, ammonia_assimilation</t>
+  </si>
+  <si>
+    <t>tetrathionate, sulfate_red_ass</t>
+  </si>
+  <si>
+    <t>a few chemotaxis protines</t>
+  </si>
+  <si>
+    <t>chitobiose, fructose, glucose, galactose, mannose, sorbitol, fructan, fucose, fuculose, rhamnose, rhamnulose, raffinose, stachyose, sucrose, manninotriose, melibiose, galactan, lactose, glycerate, cellulose, cellobiose, glucoside, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>SbmA/Bac-A-like domain, extracellular solute, iron, LPS export, lipoprotein release, molybdate, oligopeptide, phosphate, phospholipid/cholesterol, substrate-binding, sulfate</t>
+  </si>
+  <si>
+    <t>MurNAc, mannose, sucrose, glycolate, glucoside, cellobiose, maltose, starch/glycogen</t>
+  </si>
+  <si>
+    <t>MlaD, permease, amino acid/amide, arabinogalactan/maltoogliosaccharide, carbohydrate, extracellular solute, lipoprotein release, LPS transport, macrolide, molybdate, phospholipid/cholesterol, phospohnate</t>
+  </si>
+  <si>
+    <t>one carotenoid gene, partial Wood-Ljungdahl</t>
+  </si>
+  <si>
+    <t>nitroalkane, ammonia_assimilation, one nitrogen fixation subunit</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose, mannose, cellobiose, glucoside, strrch/glycogen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">branched amino, xylose, alpha-glucoside, amino acid/amide, arabinogalactan/maltooligosaccharide, biotin, carbohydrate, extracellular solute, glycine betaine/proline, iron, LPS transport, molybdate, monosaccharide, phosphate, raffinose/stachyose/melibiose, spermidine/putrescine, techoic acid, thiol reductant </t>
+  </si>
+  <si>
+    <t>two carotenoid genes, carbon fixation (RuBisCo, one gene)</t>
+  </si>
+  <si>
+    <t>glucose, galactose, galactan, lactose, raffinose, stachyose, melibiose, manninotriose, sucrose, maltose</t>
+  </si>
+  <si>
+    <t>branched amino, amino acid/amide</t>
+  </si>
+  <si>
+    <t>starch/glycogen</t>
+  </si>
+  <si>
+    <t>amino acid/amide, branched amino, carbohydrate, extracellular solute, glucose/mannose, glutathione, heme, iron(III), LPS export, microcin C, monosaccharide, multiple sugar, oligopeptide, peptide/nickel, phospholipid, raffinose/stachyose/melibiose, sn-glycerol-3-phosphate, spermidine/putrescine, sulfate, sulfonate, urea</t>
+  </si>
+  <si>
+    <t>carbon fixation (RuBisCo, 1 subunit)</t>
+  </si>
+  <si>
+    <t>thiosulfate, taurine, alkanesulfonate, methansulfonate</t>
+  </si>
+  <si>
+    <t>fructose, mannose, tartrate</t>
+  </si>
+  <si>
+    <t>permease, LPS transport, lipoprotein release, phosphate, phospholipid/cholesterol</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose, rhamnose, rhamnulose, lactose, galactan, raffinose, stachyose, manninotriose, melibiose, glycerate, glucoside, cellobiose, starch/glycogen, maltose, trehalose</t>
+  </si>
+  <si>
+    <t>LPS export, amino acid/amide, branched amino, heme, lipoprotein release, microcin C, molybdate, nitrate/nitrite, phosphate, phospholipid/cholesterol, tungstate</t>
+  </si>
+  <si>
+    <t>partial Wood-Ljungdahl, formate</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, nitrate reductase, nitrite reductase</t>
+  </si>
+  <si>
+    <t>partial sulfate_red_ass, sulfate oxidation, thiosulfate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chitobiose, glycolate, tartrate, </t>
+  </si>
+  <si>
+    <t>LPS export, permease, lipoprotein release, molybdate, peptide/nickel, phosphate, phospholipid/cholesterol, sulfate</t>
+  </si>
+  <si>
+    <t>methanol, formaldehyde, formate</t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, partial sulfate oxidation</t>
+  </si>
+  <si>
+    <t>chitobiose, MurNaC, glucose, starch/glycogen</t>
+  </si>
+  <si>
+    <t>branched amino, peptide/nickel, phosphate, sulfate</t>
+  </si>
+  <si>
+    <t>glycolate, cellobiose, glucoside</t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, partial sulfur oxidation</t>
+  </si>
+  <si>
+    <t>chitobiose, glucose, glycolate, starch/glycogen, maltose</t>
+  </si>
+  <si>
+    <t>branched amino, amino acid/amide, heme, LPS export, microcin C, molybdate, nitrate/nitrite, paraquat-inducible, phospholipid/cholesterol, tungstate</t>
+  </si>
+  <si>
+    <t>ammonia_assimilation, nitrite reductase, nitrate reductase, nitroalkane</t>
+  </si>
+  <si>
+    <t>thiosulfate, sulfur_oxidation (SOX)</t>
+  </si>
+  <si>
+    <t>chitobiose, MurNAc, glycolate, glycerate, tartrate</t>
+  </si>
+  <si>
+    <t>sulfate_red_ass, thiosulfate, alkanesulfonate, methanesulfonate</t>
+  </si>
+  <si>
+    <t>methane, methanol, formaldehyde, formate, chitobiose, MurNAc, fructose, glycolate, cellobiose, glucoside, 1,3-B-glucan, starch/glycogen, maltose</t>
   </si>
 </sst>
 </file>
@@ -3704,8 +3830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J159" workbookViewId="0">
-      <selection activeCell="M174" sqref="M174"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K189" sqref="K189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12102,6 +12228,12 @@
         <v>342</v>
       </c>
       <c r="I175" s="1"/>
+      <c r="N175" t="s">
+        <v>461</v>
+      </c>
+      <c r="T175" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="176" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
@@ -12131,11 +12263,32 @@
       <c r="I176" s="1" t="s">
         <v>500</v>
       </c>
+      <c r="J176" t="s">
+        <v>1093</v>
+      </c>
+      <c r="L176" t="s">
+        <v>1097</v>
+      </c>
       <c r="M176" t="s">
         <v>475</v>
       </c>
+      <c r="N176" t="s">
+        <v>1094</v>
+      </c>
       <c r="O176" t="s">
         <v>518</v>
+      </c>
+      <c r="P176" t="s">
+        <v>1095</v>
+      </c>
+      <c r="Q176" t="s">
+        <v>1092</v>
+      </c>
+      <c r="S176" t="s">
+        <v>1096</v>
+      </c>
+      <c r="T176" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="177" spans="1:20" x14ac:dyDescent="0.25">
@@ -12166,8 +12319,29 @@
       <c r="I177" s="1" t="s">
         <v>448</v>
       </c>
+      <c r="J177" t="s">
+        <v>596</v>
+      </c>
+      <c r="L177" t="s">
+        <v>1099</v>
+      </c>
       <c r="M177" t="s">
         <v>475</v>
+      </c>
+      <c r="N177" t="s">
+        <v>461</v>
+      </c>
+      <c r="P177" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q177" t="s">
+        <v>1098</v>
+      </c>
+      <c r="S177" t="s">
+        <v>826</v>
+      </c>
+      <c r="T177" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="178" spans="1:20" x14ac:dyDescent="0.25">
@@ -12196,6 +12370,27 @@
         <v>342</v>
       </c>
       <c r="I178" s="1"/>
+      <c r="J178" t="s">
+        <v>1101</v>
+      </c>
+      <c r="L178" t="s">
+        <v>1103</v>
+      </c>
+      <c r="N178" t="s">
+        <v>1102</v>
+      </c>
+      <c r="P178" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q178" t="s">
+        <v>1100</v>
+      </c>
+      <c r="S178" t="s">
+        <v>622</v>
+      </c>
+      <c r="T178" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="179" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
@@ -12225,8 +12420,26 @@
       <c r="I179" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="J179" t="s">
+        <v>1105</v>
+      </c>
+      <c r="L179" t="s">
+        <v>1106</v>
+      </c>
+      <c r="N179" t="s">
+        <v>694</v>
+      </c>
       <c r="O179" t="s">
         <v>510</v>
+      </c>
+      <c r="P179" t="s">
+        <v>502</v>
+      </c>
+      <c r="Q179" t="s">
+        <v>1104</v>
+      </c>
+      <c r="T179" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="180" spans="1:20" x14ac:dyDescent="0.25">
@@ -12255,6 +12468,18 @@
         <v>342</v>
       </c>
       <c r="I180" s="1"/>
+      <c r="J180" t="s">
+        <v>1108</v>
+      </c>
+      <c r="N180" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q180" t="s">
+        <v>1107</v>
+      </c>
+      <c r="T180" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="181" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
@@ -12284,11 +12509,32 @@
       <c r="I181" s="1" t="s">
         <v>449</v>
       </c>
+      <c r="J181" t="s">
+        <v>1110</v>
+      </c>
+      <c r="L181" t="s">
+        <v>1112</v>
+      </c>
       <c r="M181" t="s">
         <v>461</v>
       </c>
+      <c r="N181" t="s">
+        <v>615</v>
+      </c>
       <c r="O181" t="s">
         <v>502</v>
+      </c>
+      <c r="P181" t="s">
+        <v>1111</v>
+      </c>
+      <c r="Q181" t="s">
+        <v>1109</v>
+      </c>
+      <c r="S181" t="s">
+        <v>826</v>
+      </c>
+      <c r="T181" t="s">
+        <v>877</v>
       </c>
     </row>
     <row r="182" spans="1:20" x14ac:dyDescent="0.25">
@@ -12319,6 +12565,21 @@
       <c r="I182" s="1" t="s">
         <v>416</v>
       </c>
+      <c r="J182" t="s">
+        <v>1114</v>
+      </c>
+      <c r="N182" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q182" t="s">
+        <v>1113</v>
+      </c>
+      <c r="S182" t="s">
+        <v>604</v>
+      </c>
+      <c r="T182" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="183" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
@@ -12346,6 +12607,12 @@
         <v>342</v>
       </c>
       <c r="I183" s="1"/>
+      <c r="N183" t="s">
+        <v>461</v>
+      </c>
+      <c r="T183" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="184" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
@@ -12373,8 +12640,29 @@
         <v>342</v>
       </c>
       <c r="I184" s="1"/>
+      <c r="J184" t="s">
+        <v>1116</v>
+      </c>
       <c r="K184" t="s">
         <v>345</v>
+      </c>
+      <c r="L184" t="s">
+        <v>1119</v>
+      </c>
+      <c r="N184" t="s">
+        <v>1117</v>
+      </c>
+      <c r="P184" t="s">
+        <v>1118</v>
+      </c>
+      <c r="Q184" t="s">
+        <v>1115</v>
+      </c>
+      <c r="S184" t="s">
+        <v>604</v>
+      </c>
+      <c r="T184" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="185" spans="1:20" x14ac:dyDescent="0.25">
@@ -12405,11 +12693,29 @@
       <c r="I185" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="J185" t="s">
+        <v>1121</v>
+      </c>
+      <c r="L185" t="s">
+        <v>1123</v>
+      </c>
       <c r="M185" t="s">
         <v>471</v>
       </c>
+      <c r="N185" t="s">
+        <v>858</v>
+      </c>
       <c r="O185" t="s">
         <v>501</v>
+      </c>
+      <c r="P185" t="s">
+        <v>1122</v>
+      </c>
+      <c r="Q185" t="s">
+        <v>1120</v>
+      </c>
+      <c r="T185" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="186" spans="1:20" x14ac:dyDescent="0.25">
@@ -12438,6 +12744,21 @@
         <v>342</v>
       </c>
       <c r="I186" s="1"/>
+      <c r="J186" t="s">
+        <v>1125</v>
+      </c>
+      <c r="N186" t="s">
+        <v>461</v>
+      </c>
+      <c r="P186" t="s">
+        <v>653</v>
+      </c>
+      <c r="Q186" t="s">
+        <v>1124</v>
+      </c>
+      <c r="T186" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="187" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
@@ -12467,8 +12788,26 @@
       <c r="I187" s="1" t="s">
         <v>390</v>
       </c>
+      <c r="J187" t="s">
+        <v>1121</v>
+      </c>
+      <c r="L187" t="s">
+        <v>1127</v>
+      </c>
       <c r="M187" t="s">
         <v>471</v>
+      </c>
+      <c r="N187" t="s">
+        <v>858</v>
+      </c>
+      <c r="P187" t="s">
+        <v>1126</v>
+      </c>
+      <c r="Q187" t="s">
+        <v>857</v>
+      </c>
+      <c r="T187" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="188" spans="1:20" x14ac:dyDescent="0.25">
@@ -12499,11 +12838,29 @@
       <c r="I188" s="1" t="s">
         <v>437</v>
       </c>
+      <c r="J188" t="s">
+        <v>1131</v>
+      </c>
       <c r="M188" t="s">
         <v>475</v>
       </c>
+      <c r="N188" t="s">
+        <v>1129</v>
+      </c>
       <c r="O188" t="s">
         <v>510</v>
+      </c>
+      <c r="P188" t="s">
+        <v>1130</v>
+      </c>
+      <c r="Q188" t="s">
+        <v>1128</v>
+      </c>
+      <c r="S188" t="s">
+        <v>994</v>
+      </c>
+      <c r="T188" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="189" spans="1:20" x14ac:dyDescent="0.25">
@@ -12534,11 +12891,26 @@
       <c r="I189" s="1" t="s">
         <v>450</v>
       </c>
+      <c r="J189" t="s">
+        <v>1133</v>
+      </c>
       <c r="M189" t="s">
         <v>461</v>
       </c>
+      <c r="N189" t="s">
+        <v>917</v>
+      </c>
       <c r="O189" t="s">
         <v>502</v>
+      </c>
+      <c r="P189" t="s">
+        <v>1132</v>
+      </c>
+      <c r="Q189" t="s">
+        <v>836</v>
+      </c>
+      <c r="T189" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="190" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Got feedback from Trina
</commit_message>
<xml_diff>
--- a/Data_files/combined_genome_data.xlsx
+++ b/Data_files/combined_genome_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\MAGstravaganza\Data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amlin\Desktop\MAGstravaganza\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2328" uniqueCount="1089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2354" uniqueCount="1094">
   <si>
     <t>ME</t>
   </si>
@@ -3291,12 +3291,27 @@
   </si>
   <si>
     <t>iron(III), phosphate, phospholipid, spermidine/putrescine, sulfate, zinc, fructose, NAG, PEP-protein</t>
+  </si>
+  <si>
+    <t>Operon_check</t>
+  </si>
+  <si>
+    <t>n.fix</t>
+  </si>
+  <si>
+    <t>NO.n.fix</t>
+  </si>
+  <si>
+    <t>n.fix(in 2nd operon, small contig?)</t>
+  </si>
+  <si>
+    <t>borderline.n.fix</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3667,10 +3682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R206"/>
+  <dimension ref="A1:S206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3688,9 +3703,10 @@
     <col min="12" max="12" width="37.140625" customWidth="1"/>
     <col min="13" max="13" width="5.5703125" customWidth="1"/>
     <col min="17" max="17" width="13.140625" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
@@ -3745,8 +3761,11 @@
       <c r="R1" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2582580512</v>
       </c>
@@ -3793,7 +3812,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>498</v>
       </c>
@@ -3837,7 +3856,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2582580514</v>
       </c>
@@ -3878,7 +3897,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2582580515</v>
       </c>
@@ -3925,7 +3944,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2582580516</v>
       </c>
@@ -3969,7 +3988,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2582580517</v>
       </c>
@@ -4016,7 +4035,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>517</v>
       </c>
@@ -4065,8 +4084,11 @@
       <c r="Q8" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2582580519</v>
       </c>
@@ -4113,7 +4135,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2582580520</v>
       </c>
@@ -4154,7 +4176,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2582580521</v>
       </c>
@@ -4204,7 +4226,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2582580522</v>
       </c>
@@ -4254,7 +4276,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2582580523</v>
       </c>
@@ -4304,7 +4326,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2582580524</v>
       </c>
@@ -4354,7 +4376,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2582580525</v>
       </c>
@@ -4401,7 +4423,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2582580526</v>
       </c>
@@ -4445,7 +4467,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2582580527</v>
       </c>
@@ -4489,7 +4511,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2582580528</v>
       </c>
@@ -4530,7 +4552,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2582580529</v>
       </c>
@@ -4577,7 +4599,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2582580530</v>
       </c>
@@ -4618,7 +4640,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2582580531</v>
       </c>
@@ -4668,7 +4690,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2582580532</v>
       </c>
@@ -4718,7 +4740,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2582580533</v>
       </c>
@@ -4762,7 +4784,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2582580534</v>
       </c>
@@ -4803,7 +4825,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2582580535</v>
       </c>
@@ -4853,7 +4875,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2582580536</v>
       </c>
@@ -4903,7 +4925,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2582580537</v>
       </c>
@@ -4952,8 +4974,11 @@
       <c r="R27" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S27" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2582580538</v>
       </c>
@@ -5003,7 +5028,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2582580539</v>
       </c>
@@ -5041,7 +5066,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2582580540</v>
       </c>
@@ -5094,7 +5119,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2582580541</v>
       </c>
@@ -5141,7 +5166,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2582580542</v>
       </c>
@@ -5188,7 +5213,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2582580543</v>
       </c>
@@ -5227,7 +5252,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2582580544</v>
       </c>
@@ -5271,7 +5296,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2582580545</v>
       </c>
@@ -5312,7 +5337,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2582580546</v>
       </c>
@@ -5356,7 +5381,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2582580547</v>
       </c>
@@ -5406,7 +5431,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2582580548</v>
       </c>
@@ -5456,7 +5481,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2582580549</v>
       </c>
@@ -5500,7 +5525,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2582580550</v>
       </c>
@@ -5547,7 +5572,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2582580551</v>
       </c>
@@ -5597,7 +5622,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2582580552</v>
       </c>
@@ -5646,8 +5671,11 @@
       <c r="R42" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S42" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2582580553</v>
       </c>
@@ -5686,7 +5714,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>2582580554</v>
       </c>
@@ -5731,7 +5759,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2582580555</v>
       </c>
@@ -5766,7 +5794,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>2582580556</v>
       </c>
@@ -5819,7 +5847,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>2582580557</v>
       </c>
@@ -5864,7 +5892,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>2582580558</v>
       </c>
@@ -5911,7 +5939,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>2582580559</v>
       </c>
@@ -5952,7 +5980,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>2582580560</v>
       </c>
@@ -6002,7 +6030,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>2582580561</v>
       </c>
@@ -6052,7 +6080,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>2582580562</v>
       </c>
@@ -6088,7 +6116,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>2582580563</v>
       </c>
@@ -6133,7 +6161,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>2582580564</v>
       </c>
@@ -6177,7 +6205,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>2582580565</v>
       </c>
@@ -6227,7 +6255,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>2582580566</v>
       </c>
@@ -6280,7 +6308,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>2582580567</v>
       </c>
@@ -6323,8 +6351,11 @@
       <c r="R57" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="58" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S57" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>2582580568</v>
       </c>
@@ -6371,7 +6402,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="59" spans="1:18" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>2582580569</v>
       </c>
@@ -6420,7 +6451,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>2582580571</v>
       </c>
@@ -6464,7 +6495,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>2582580572</v>
       </c>
@@ -6505,7 +6536,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>2582580573</v>
       </c>
@@ -6546,7 +6577,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>2582580574</v>
       </c>
@@ -6590,7 +6621,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>2582580575</v>
       </c>
@@ -6634,7 +6665,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>2582580576</v>
       </c>
@@ -6684,7 +6715,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>2582580577</v>
       </c>
@@ -6731,7 +6762,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>2582580578</v>
       </c>
@@ -6784,7 +6815,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>2582580579</v>
       </c>
@@ -6822,7 +6853,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>2582580580</v>
       </c>
@@ -6863,7 +6894,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>2582580581</v>
       </c>
@@ -6910,7 +6941,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>2582580582</v>
       </c>
@@ -6951,7 +6982,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>2582580583</v>
       </c>
@@ -6992,7 +7023,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>2582580584</v>
       </c>
@@ -7035,8 +7066,11 @@
       <c r="R73" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S73" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>2582580585</v>
       </c>
@@ -7083,7 +7117,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>2582580586</v>
       </c>
@@ -7127,7 +7161,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>2582580587</v>
       </c>
@@ -7169,7 +7203,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>2582580588</v>
       </c>
@@ -7210,7 +7244,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>2582580589</v>
       </c>
@@ -7260,7 +7294,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>2582580590</v>
       </c>
@@ -7298,7 +7332,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>2582580591</v>
       </c>
@@ -8084,7 +8118,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>2582580608</v>
       </c>
@@ -8125,7 +8159,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>2582580609</v>
       </c>
@@ -8172,7 +8206,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>2582580610</v>
       </c>
@@ -8214,7 +8248,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>2582580611</v>
       </c>
@@ -8261,7 +8295,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>2582580612</v>
       </c>
@@ -8303,7 +8337,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>2582580613</v>
       </c>
@@ -8347,7 +8381,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>2582580614</v>
       </c>
@@ -8394,7 +8428,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>2582580615</v>
       </c>
@@ -8447,7 +8481,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>2582580616</v>
       </c>
@@ -8492,7 +8526,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>2582580617</v>
       </c>
@@ -8531,7 +8565,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>2582580620</v>
       </c>
@@ -8581,7 +8615,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>2582580621</v>
       </c>
@@ -8631,7 +8665,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>2582580622</v>
       </c>
@@ -8683,8 +8717,11 @@
       <c r="R109" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S109" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>2582580623</v>
       </c>
@@ -8731,7 +8768,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>2582580624</v>
       </c>
@@ -8776,7 +8813,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>2582580625</v>
       </c>
@@ -8820,6 +8857,9 @@
       <c r="R112" t="s">
         <v>523</v>
       </c>
+      <c r="S112" t="s">
+        <v>1090</v>
+      </c>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
@@ -9551,7 +9591,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>2582580644</v>
       </c>
@@ -9590,7 +9630,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>2582580646</v>
       </c>
@@ -9639,8 +9679,11 @@
       <c r="R130" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S130" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>2582580647</v>
       </c>
@@ -9684,7 +9727,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>2582580648</v>
       </c>
@@ -9736,8 +9779,11 @@
       <c r="R132" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S132" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>2582580649</v>
       </c>
@@ -9784,7 +9830,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>2582580650</v>
       </c>
@@ -9834,7 +9880,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>2582580651</v>
       </c>
@@ -9886,8 +9932,11 @@
       <c r="R135" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S135" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>2582580652</v>
       </c>
@@ -9922,7 +9971,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>2582580653</v>
       </c>
@@ -9969,7 +10018,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>2582580654</v>
       </c>
@@ -10021,8 +10070,11 @@
       <c r="R138" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S138" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>2582580657</v>
       </c>
@@ -10069,7 +10121,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>2582580658</v>
       </c>
@@ -10118,8 +10170,11 @@
       <c r="R140" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S140" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>2582580659</v>
       </c>
@@ -10171,8 +10226,11 @@
       <c r="R141" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S141" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>2582580662</v>
       </c>
@@ -10221,8 +10279,11 @@
       <c r="R142" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S142" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>2582580663</v>
       </c>
@@ -10255,7 +10316,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>2582580664</v>
       </c>
@@ -10305,7 +10366,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>2582580665</v>
       </c>
@@ -10354,8 +10415,11 @@
       <c r="R145" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S145" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>2582580668</v>
       </c>
@@ -10405,7 +10469,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>2582580669</v>
       </c>
@@ -10458,7 +10522,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>2582580670</v>
       </c>
@@ -10502,7 +10566,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>2582580671</v>
       </c>
@@ -10546,7 +10610,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>2582580672</v>
       </c>
@@ -10599,7 +10663,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>2582580673</v>
       </c>
@@ -10649,7 +10713,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>2582580674</v>
       </c>
@@ -10699,7 +10763,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>2582580675</v>
       </c>
@@ -10743,7 +10807,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>2582580677</v>
       </c>
@@ -10792,8 +10856,11 @@
       <c r="R154" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S154" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>2582580679</v>
       </c>
@@ -10832,7 +10899,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>2582580680</v>
       </c>
@@ -10878,8 +10945,11 @@
       <c r="R156" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S156" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>2582580682</v>
       </c>
@@ -10925,8 +10995,11 @@
       <c r="R157" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S157" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>2582580683</v>
       </c>
@@ -10968,7 +11041,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>2582580684</v>
       </c>
@@ -11015,8 +11088,11 @@
       <c r="R159" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S159" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>2582580685</v>
       </c>
@@ -11060,7 +11136,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>2582580686</v>
       </c>
@@ -11101,7 +11177,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>2582580687</v>
       </c>
@@ -11154,7 +11230,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>2582580688</v>
       </c>
@@ -11201,7 +11277,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>2582580689</v>
       </c>
@@ -11253,8 +11329,11 @@
       <c r="R164" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S164" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>2582580690</v>
       </c>
@@ -11298,7 +11377,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>2582580691</v>
       </c>
@@ -11351,7 +11430,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>2582580692</v>
       </c>
@@ -11400,8 +11479,11 @@
       <c r="R167" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S167" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>2582580693</v>
       </c>
@@ -11434,7 +11516,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>2582580694</v>
       </c>
@@ -11479,7 +11561,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>2582580695</v>
       </c>
@@ -11532,7 +11614,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>2582580697</v>
       </c>
@@ -11585,7 +11667,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>2582580698</v>
       </c>
@@ -11624,7 +11706,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>2582580699</v>
       </c>
@@ -11669,7 +11751,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>2582580700</v>
       </c>
@@ -11719,7 +11801,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>2582580701</v>
       </c>
@@ -11752,7 +11834,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>2582580702</v>
       </c>
@@ -11805,7 +11887,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>2582580703</v>
       </c>
@@ -11855,7 +11937,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>2582580704</v>
       </c>
@@ -11899,8 +11981,11 @@
       <c r="R178" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S178" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="179" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>2582580705</v>
       </c>
@@ -11947,7 +12032,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>2582580706</v>
       </c>
@@ -11986,7 +12071,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="181" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>2582580707</v>
       </c>
@@ -12039,7 +12124,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>2582580708</v>
       </c>
@@ -12083,7 +12168,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="183" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>2582580709</v>
       </c>
@@ -12116,7 +12201,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="184" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>2582580711</v>
       </c>
@@ -12163,7 +12248,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="185" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>2582580712</v>
       </c>
@@ -12213,7 +12298,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>2582580714</v>
       </c>
@@ -12255,7 +12340,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="187" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>2593339176</v>
       </c>
@@ -12302,7 +12387,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="188" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>2593339177</v>
       </c>
@@ -12355,7 +12440,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="189" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>2593339178</v>
       </c>
@@ -12404,8 +12489,11 @@
       <c r="R189" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="190" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S189" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="190" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>2593339179</v>
       </c>
@@ -12458,7 +12546,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>2593339181</v>
       </c>
@@ -12502,7 +12590,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="192" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>2593339182</v>
       </c>
@@ -12544,7 +12632,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="193" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>2593339183</v>
       </c>
@@ -12593,8 +12681,11 @@
       <c r="R193" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="194" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S193" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="194" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>2593339184</v>
       </c>
@@ -12646,8 +12737,11 @@
       <c r="R194" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="195" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S194" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="195" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>2593339185</v>
       </c>
@@ -12691,7 +12785,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="196" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>2593339186</v>
       </c>
@@ -12730,7 +12824,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="197" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>2593339187</v>
       </c>
@@ -12780,7 +12874,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="198" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>2593339188</v>
       </c>
@@ -12822,7 +12916,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="199" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>2593339189</v>
       </c>
@@ -12866,7 +12960,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="200" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>2593339190</v>
       </c>
@@ -12905,7 +12999,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>2593339191</v>
       </c>
@@ -12955,7 +13049,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="202" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>2593339192</v>
       </c>
@@ -12999,7 +13093,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>2593339193</v>
       </c>
@@ -13046,13 +13140,13 @@
         <v>523</v>
       </c>
     </row>
-    <row r="204" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:19" x14ac:dyDescent="0.25">
       <c r="I204" s="1"/>
     </row>
-    <row r="205" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:19" x14ac:dyDescent="0.25">
       <c r="I205" s="1"/>
     </row>
-    <row r="206" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:19" x14ac:dyDescent="0.25">
       <c r="I206" s="1"/>
     </row>
   </sheetData>

</xml_diff>